<commit_message>
Upload results for biofuel and biomass shocks
- 1000 MC trials
</commit_message>
<xml_diff>
--- a/results/xlsx/KDI_results.xlsx
+++ b/results/xlsx/KDI_results.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="682" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="gasoline_shocks" sheetId="3" r:id="rId1"/>
+    <sheet name="fuel_shocks" sheetId="3" r:id="rId1"/>
     <sheet name="electricity_shocks" sheetId="4" r:id="rId2"/>
-    <sheet name="gasoline_shocks_MC_trials" sheetId="6" r:id="rId3"/>
+    <sheet name="fuel_shocks_MC_trials" sheetId="6" r:id="rId3"/>
     <sheet name="electricity_shocks_MC_trials" sheetId="7" r:id="rId4"/>
+    <sheet name="electricity_percent_shocks" sheetId="8" r:id="rId5"/>
+    <sheet name="fuel_percent_shocks" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
@@ -137,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="56">
   <si>
     <t>Feedstock</t>
   </si>
@@ -304,6 +306,15 @@
   <si>
     <t>95th Percentile</t>
   </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>% Quantity Change    Gasoline</t>
+  </si>
+  <si>
+    <t>Rebound effect on Gasoline</t>
+  </si>
 </sst>
 </file>
 
@@ -314,7 +325,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000000000000%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,8 +392,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +411,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCB5151"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -437,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -483,11 +519,41 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="61">
+    <dxf>
+      <border>
+        <left style="dashDotDot">
+          <color auto="1"/>
+        </left>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000%"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -549,19 +615,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="0.000%"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -573,6 +626,19 @@
         <shadow val="0"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -914,34 +980,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:O20" totalsRowShown="0" headerRowDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:O20" totalsRowShown="0" headerRowDxfId="60">
   <autoFilter ref="A1:O20"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Feedstock" dataDxfId="58"/>
+    <tableColumn id="1" name="Feedstock" dataDxfId="59"/>
     <tableColumn id="2" name="Technology"/>
     <tableColumn id="3" name="Quantity (MatLab)"/>
     <tableColumn id="4" name="Unit"/>
     <tableColumn id="14" name="Notes"/>
-    <tableColumn id="16" name="% Supply Shock" dataDxfId="57"/>
-    <tableColumn id="5" name="% Price Change_x000a_Fuel" dataDxfId="56"/>
-    <tableColumn id="6" name="% Price Change_x000a_Electricity" dataDxfId="55"/>
-    <tableColumn id="7" name="% Price Change_x000a_Natural Gas" dataDxfId="54"/>
-    <tableColumn id="8" name="% Quantity Change_x000a_Fuel" dataDxfId="53"/>
-    <tableColumn id="9" name="% Quantity Change_x000a_Electricity" dataDxfId="52"/>
-    <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas" dataDxfId="51"/>
-    <tableColumn id="11" name="% Quantity Change_x000a_Gasoline" dataDxfId="50"/>
-    <tableColumn id="19" name="Rebound Effect    Gasoline" dataDxfId="49"/>
-    <tableColumn id="15" name="CO2 Reduction (tonnes)" dataDxfId="48"/>
+    <tableColumn id="16" name="% Supply Shock" dataDxfId="58"/>
+    <tableColumn id="5" name="% Price Change_x000a_Fuel" dataDxfId="57"/>
+    <tableColumn id="6" name="% Price Change_x000a_Electricity" dataDxfId="56"/>
+    <tableColumn id="7" name="% Price Change_x000a_Natural Gas" dataDxfId="55"/>
+    <tableColumn id="8" name="% Quantity Change_x000a_Fuel" dataDxfId="54"/>
+    <tableColumn id="9" name="% Quantity Change_x000a_Electricity" dataDxfId="53"/>
+    <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas" dataDxfId="52"/>
+    <tableColumn id="11" name="% Quantity Change_x000a_Gasoline" dataDxfId="51"/>
+    <tableColumn id="19" name="Rebound Effect    Gasoline" dataDxfId="50"/>
+    <tableColumn id="15" name="CO2 Reduction (tonnes)" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table36" displayName="Table36" ref="A1:O38" totalsRowShown="0" headerRowDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table36" displayName="Table36" ref="A1:O38" totalsRowShown="0" headerRowDxfId="48">
   <autoFilter ref="A1:O38"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Feedstock" dataDxfId="46"/>
+    <tableColumn id="1" name="Feedstock" dataDxfId="47"/>
     <tableColumn id="2" name="Technology"/>
     <tableColumn id="3" name="Quantity (MatLab)"/>
     <tableColumn id="4" name="Unit"/>
@@ -954,7 +1020,7 @@
     <tableColumn id="9" name="% Quantity Change_x000a_Electricity"/>
     <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas"/>
     <tableColumn id="12" name="% Quantity Change    Non-biomass Electricity"/>
-    <tableColumn id="18" name="Rebound effect on Electricity" dataDxfId="45"/>
+    <tableColumn id="18" name="Rebound effect on Electricity" dataDxfId="46"/>
     <tableColumn id="14" name="CO2 Reduction (tonnes)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -962,79 +1028,79 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table33" displayName="Table33" ref="A2:O21" totalsRowShown="0" headerRowDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table33" displayName="Table33" ref="A2:O21" totalsRowShown="0" headerRowDxfId="45">
   <autoFilter ref="A2:O21"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Feedstock" dataDxfId="43"/>
+    <tableColumn id="1" name="Feedstock" dataDxfId="44"/>
     <tableColumn id="2" name="Technology"/>
     <tableColumn id="3" name="Quantity (MatLab)"/>
     <tableColumn id="4" name="Unit"/>
     <tableColumn id="14" name="Notes"/>
-    <tableColumn id="16" name="% Supply Shock" dataDxfId="42"/>
-    <tableColumn id="5" name="% Price Change_x000a_Fuel" dataDxfId="41"/>
-    <tableColumn id="6" name="% Price Change_x000a_Electricity" dataDxfId="40"/>
-    <tableColumn id="7" name="% Price Change_x000a_Natural Gas" dataDxfId="39"/>
-    <tableColumn id="8" name="% Quantity Change_x000a_Fuel" dataDxfId="38"/>
-    <tableColumn id="9" name="% Quantity Change_x000a_Electricity" dataDxfId="37"/>
-    <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas" dataDxfId="36"/>
-    <tableColumn id="11" name="% Quantity Change_x000a_Gasoline" dataDxfId="35"/>
-    <tableColumn id="19" name="Rebound Effect    Gasoline" dataDxfId="34"/>
-    <tableColumn id="15" name="CO2 Reduction (tonnes)" dataDxfId="33"/>
+    <tableColumn id="16" name="% Supply Shock" dataDxfId="43"/>
+    <tableColumn id="5" name="% Price Change_x000a_Fuel" dataDxfId="42"/>
+    <tableColumn id="6" name="% Price Change_x000a_Electricity" dataDxfId="41"/>
+    <tableColumn id="7" name="% Price Change_x000a_Natural Gas" dataDxfId="40"/>
+    <tableColumn id="8" name="% Quantity Change_x000a_Fuel" dataDxfId="39"/>
+    <tableColumn id="9" name="% Quantity Change_x000a_Electricity" dataDxfId="38"/>
+    <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas" dataDxfId="37"/>
+    <tableColumn id="11" name="% Quantity Change_x000a_Gasoline" dataDxfId="36"/>
+    <tableColumn id="19" name="Rebound Effect    Gasoline" dataDxfId="35"/>
+    <tableColumn id="15" name="CO2 Reduction (tonnes)" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table336" displayName="Table336" ref="A25:O44" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table336" displayName="Table336" ref="A25:O44" totalsRowShown="0" headerRowDxfId="33">
   <autoFilter ref="A25:O44"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Feedstock" dataDxfId="31"/>
+    <tableColumn id="1" name="Feedstock" dataDxfId="32"/>
     <tableColumn id="2" name="Technology"/>
     <tableColumn id="3" name="Quantity (MatLab)"/>
     <tableColumn id="4" name="Unit"/>
     <tableColumn id="14" name="Notes"/>
-    <tableColumn id="16" name="% Supply Shock" dataDxfId="30"/>
-    <tableColumn id="5" name="% Price Change_x000a_Fuel" dataDxfId="29"/>
-    <tableColumn id="6" name="% Price Change_x000a_Electricity" dataDxfId="28"/>
-    <tableColumn id="7" name="% Price Change_x000a_Natural Gas" dataDxfId="27"/>
-    <tableColumn id="8" name="% Quantity Change_x000a_Fuel" dataDxfId="26"/>
-    <tableColumn id="9" name="% Quantity Change_x000a_Electricity" dataDxfId="25"/>
-    <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas" dataDxfId="24"/>
-    <tableColumn id="11" name="% Quantity Change_x000a_Gasoline" dataDxfId="23"/>
-    <tableColumn id="19" name="Rebound Effect    Gasoline" dataDxfId="22"/>
-    <tableColumn id="15" name="CO2 Reduction (tonnes)" dataDxfId="21"/>
+    <tableColumn id="16" name="% Supply Shock" dataDxfId="31"/>
+    <tableColumn id="5" name="% Price Change_x000a_Fuel" dataDxfId="30"/>
+    <tableColumn id="6" name="% Price Change_x000a_Electricity" dataDxfId="29"/>
+    <tableColumn id="7" name="% Price Change_x000a_Natural Gas" dataDxfId="28"/>
+    <tableColumn id="8" name="% Quantity Change_x000a_Fuel" dataDxfId="27"/>
+    <tableColumn id="9" name="% Quantity Change_x000a_Electricity" dataDxfId="26"/>
+    <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas" dataDxfId="25"/>
+    <tableColumn id="11" name="% Quantity Change_x000a_Gasoline" dataDxfId="24"/>
+    <tableColumn id="19" name="Rebound Effect    Gasoline" dataDxfId="23"/>
+    <tableColumn id="15" name="CO2 Reduction (tonnes)" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table3367" displayName="Table3367" ref="A48:O67" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table3367" displayName="Table3367" ref="A48:O67" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="A48:O67"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Feedstock" dataDxfId="19"/>
+    <tableColumn id="1" name="Feedstock" dataDxfId="20"/>
     <tableColumn id="2" name="Technology"/>
     <tableColumn id="3" name="Quantity (MatLab)"/>
     <tableColumn id="4" name="Unit"/>
     <tableColumn id="14" name="Notes"/>
-    <tableColumn id="16" name="% Supply Shock" dataDxfId="18"/>
-    <tableColumn id="5" name="% Price Change_x000a_Fuel" dataDxfId="17"/>
-    <tableColumn id="6" name="% Price Change_x000a_Electricity" dataDxfId="16"/>
-    <tableColumn id="7" name="% Price Change_x000a_Natural Gas" dataDxfId="15"/>
-    <tableColumn id="8" name="% Quantity Change_x000a_Fuel" dataDxfId="14"/>
-    <tableColumn id="9" name="% Quantity Change_x000a_Electricity" dataDxfId="13"/>
-    <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas" dataDxfId="12"/>
-    <tableColumn id="11" name="% Quantity Change_x000a_Gasoline" dataDxfId="11"/>
-    <tableColumn id="19" name="Rebound Effect    Gasoline" dataDxfId="10"/>
-    <tableColumn id="15" name="CO2 Reduction (tonnes)" dataDxfId="9"/>
+    <tableColumn id="16" name="% Supply Shock" dataDxfId="19"/>
+    <tableColumn id="5" name="% Price Change_x000a_Fuel" dataDxfId="18"/>
+    <tableColumn id="6" name="% Price Change_x000a_Electricity" dataDxfId="17"/>
+    <tableColumn id="7" name="% Price Change_x000a_Natural Gas" dataDxfId="16"/>
+    <tableColumn id="8" name="% Quantity Change_x000a_Fuel" dataDxfId="15"/>
+    <tableColumn id="9" name="% Quantity Change_x000a_Electricity" dataDxfId="14"/>
+    <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas" dataDxfId="13"/>
+    <tableColumn id="11" name="% Quantity Change_x000a_Gasoline" dataDxfId="12"/>
+    <tableColumn id="19" name="Rebound Effect    Gasoline" dataDxfId="11"/>
+    <tableColumn id="15" name="CO2 Reduction (tonnes)" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table368" displayName="Table368" ref="A2:O39" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table368" displayName="Table368" ref="A2:O39" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A2:O39"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Feedstock" dataDxfId="8"/>
@@ -1058,10 +1124,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table3689" displayName="Table3689" ref="A43:O80" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table3689" displayName="Table3689" ref="A43:O80" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A43:O80"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Feedstock" dataDxfId="4"/>
+    <tableColumn id="1" name="Feedstock" dataDxfId="5"/>
     <tableColumn id="2" name="Technology"/>
     <tableColumn id="3" name="Quantity (MatLab)"/>
     <tableColumn id="4" name="Unit"/>
@@ -1074,7 +1140,7 @@
     <tableColumn id="9" name="% Quantity Change_x000a_Electricity"/>
     <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas"/>
     <tableColumn id="12" name="% Quantity Change    Non-biomass Electricity"/>
-    <tableColumn id="18" name="Rebound effect on Electricity" dataDxfId="3"/>
+    <tableColumn id="18" name="Rebound effect on Electricity" dataDxfId="4"/>
     <tableColumn id="14" name="CO2 Reduction (tonnes)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1082,10 +1148,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table36810" displayName="Table36810" ref="A84:O121" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table36810" displayName="Table36810" ref="A84:O121" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A84:O121"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Feedstock" dataDxfId="1"/>
+    <tableColumn id="1" name="Feedstock" dataDxfId="2"/>
     <tableColumn id="2" name="Technology"/>
     <tableColumn id="3" name="Quantity (MatLab)"/>
     <tableColumn id="4" name="Unit"/>
@@ -1098,7 +1164,7 @@
     <tableColumn id="9" name="% Quantity Change_x000a_Electricity"/>
     <tableColumn id="10" name="% Quantity Change_x000a_Natural Gas"/>
     <tableColumn id="12" name="% Quantity Change    Non-biomass Electricity"/>
-    <tableColumn id="18" name="Rebound effect on Electricity" dataDxfId="0"/>
+    <tableColumn id="18" name="Rebound effect on Electricity" dataDxfId="1"/>
     <tableColumn id="14" name="CO2 Reduction (tonnes)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1396,7 +1462,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1:O13"/>
+      <selection pane="topRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6877,8 +6943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView topLeftCell="E31" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12335,4 +12401,4372 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J73"/>
+  <sheetViews>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:J48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="7" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="10" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="B4" s="26">
+        <v>-3.2326958676073899E-3</v>
+      </c>
+      <c r="C4" s="26">
+        <v>-0.15553254562347699</v>
+      </c>
+      <c r="D4" s="26">
+        <v>-4.0331732381847903E-2</v>
+      </c>
+      <c r="E4" s="26">
+        <v>-9.3748180160617303E-4</v>
+      </c>
+      <c r="F4" s="26">
+        <v>3.9112721806356603E-2</v>
+      </c>
+      <c r="G4" s="26">
+        <v>-2.0165866190923901E-3</v>
+      </c>
+      <c r="H4" s="26">
+        <v>-1.03688363748985E-2</v>
+      </c>
+      <c r="I4" s="26">
+        <v>0.79262327250203102</v>
+      </c>
+      <c r="J4" s="27">
+        <v>66.830711933885496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
+        <f>A4+5%</f>
+        <v>0.1</v>
+      </c>
+      <c r="B5" s="28">
+        <v>-6.4653917352148404E-3</v>
+      </c>
+      <c r="C5" s="28">
+        <v>-0.31106509124695497</v>
+      </c>
+      <c r="D5" s="28">
+        <v>-8.0663464763695805E-2</v>
+      </c>
+      <c r="E5" s="28">
+        <v>-1.87496360321234E-3</v>
+      </c>
+      <c r="F5" s="28">
+        <v>7.8225443612713205E-2</v>
+      </c>
+      <c r="G5" s="28">
+        <v>-4.0331732381847897E-3</v>
+      </c>
+      <c r="H5" s="28">
+        <v>-1.9795051261169799E-2</v>
+      </c>
+      <c r="I5" s="28">
+        <v>0.80204948738830195</v>
+      </c>
+      <c r="J5" s="29">
+        <v>133.66142386777099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <f t="shared" ref="A6:A13" si="0">A5+5%</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="B6" s="26">
+        <v>-9.6980876028222793E-3</v>
+      </c>
+      <c r="C6" s="26">
+        <v>-0.46659763687043099</v>
+      </c>
+      <c r="D6" s="26">
+        <v>-0.12099519714554401</v>
+      </c>
+      <c r="E6" s="26">
+        <v>-2.8124454048184902E-3</v>
+      </c>
+      <c r="F6" s="26">
+        <v>0.11733816541907</v>
+      </c>
+      <c r="G6" s="26">
+        <v>-6.0497598572771703E-3</v>
+      </c>
+      <c r="H6" s="26">
+        <v>-2.8401595287765501E-2</v>
+      </c>
+      <c r="I6" s="26">
+        <v>0.81065603141489695</v>
+      </c>
+      <c r="J6" s="27">
+        <v>200.49213580165701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="B7" s="28">
+        <v>-1.29307834704297E-2</v>
+      </c>
+      <c r="C7" s="28">
+        <v>-0.62213018249390895</v>
+      </c>
+      <c r="D7" s="28">
+        <v>-0.161326929527391</v>
+      </c>
+      <c r="E7" s="28">
+        <v>-3.7499272064246401E-3</v>
+      </c>
+      <c r="F7" s="28">
+        <v>0.15645088722542599</v>
+      </c>
+      <c r="G7" s="28">
+        <v>-8.0663464763695708E-3</v>
+      </c>
+      <c r="H7" s="28">
+        <v>-3.6290927312144797E-2</v>
+      </c>
+      <c r="I7" s="28">
+        <v>0.81854536343927597</v>
+      </c>
+      <c r="J7" s="29">
+        <v>267.32284773554301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="B8" s="26">
+        <v>-1.61634793380371E-2</v>
+      </c>
+      <c r="C8" s="26">
+        <v>-0.77766272811738901</v>
+      </c>
+      <c r="D8" s="26">
+        <v>-0.20165866190924001</v>
+      </c>
+      <c r="E8" s="26">
+        <v>-4.6874090080308E-3</v>
+      </c>
+      <c r="F8" s="26">
+        <v>0.19556360903178299</v>
+      </c>
+      <c r="G8" s="26">
+        <v>-1.0082933095462E-2</v>
+      </c>
+      <c r="H8" s="26">
+        <v>-4.3549112774573601E-2</v>
+      </c>
+      <c r="I8" s="26">
+        <v>0.82580354890170504</v>
+      </c>
+      <c r="J8" s="27">
+        <v>334.15355966942798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="B9" s="28">
+        <v>-1.93961752056446E-2</v>
+      </c>
+      <c r="C9" s="28">
+        <v>-0.93319527374086497</v>
+      </c>
+      <c r="D9" s="28">
+        <v>-0.24199039429108701</v>
+      </c>
+      <c r="E9" s="28">
+        <v>-5.6248908096369604E-3</v>
+      </c>
+      <c r="F9" s="28">
+        <v>0.23467633083813899</v>
+      </c>
+      <c r="G9" s="28">
+        <v>-1.20995197145544E-2</v>
+      </c>
+      <c r="H9" s="28">
+        <v>-5.0248976278354403E-2</v>
+      </c>
+      <c r="I9" s="28">
+        <v>0.83250341240548598</v>
+      </c>
+      <c r="J9" s="29">
+        <v>400.98427160331403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="32">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="B10" s="26">
+        <v>-2.2628871073252E-2</v>
+      </c>
+      <c r="C10" s="26">
+        <v>-1.0887278193643399</v>
+      </c>
+      <c r="D10" s="26">
+        <v>-0.28232212667293499</v>
+      </c>
+      <c r="E10" s="26">
+        <v>-6.5623726112431103E-3</v>
+      </c>
+      <c r="F10" s="26">
+        <v>0.27378905264449599</v>
+      </c>
+      <c r="G10" s="26">
+        <v>-1.4116106333646799E-2</v>
+      </c>
+      <c r="H10" s="26">
+        <v>-5.6452553596669702E-2</v>
+      </c>
+      <c r="I10" s="26">
+        <v>0.83870698972379898</v>
+      </c>
+      <c r="J10" s="27">
+        <v>467.81498353720002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="B11" s="28">
+        <v>-2.58615669408594E-2</v>
+      </c>
+      <c r="C11" s="28">
+        <v>-1.2442603649878199</v>
+      </c>
+      <c r="D11" s="28">
+        <v>-0.322653859054783</v>
+      </c>
+      <c r="E11" s="28">
+        <v>-7.4998544128492602E-3</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0.31290177445085299</v>
+      </c>
+      <c r="G11" s="28">
+        <v>-1.6132692952739201E-2</v>
+      </c>
+      <c r="H11" s="28">
+        <v>-6.2213018249391003E-2</v>
+      </c>
+      <c r="I11" s="28">
+        <v>0.84446745437652104</v>
+      </c>
+      <c r="J11" s="29">
+        <v>534.64569547108499</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="B12" s="26">
+        <v>-2.90942628084668E-2</v>
+      </c>
+      <c r="C12" s="26">
+        <v>-1.3997929106113001</v>
+      </c>
+      <c r="D12" s="26">
+        <v>-0.36298559143663101</v>
+      </c>
+      <c r="E12" s="26">
+        <v>-8.4373362144554206E-3</v>
+      </c>
+      <c r="F12" s="26">
+        <v>0.35201449625720899</v>
+      </c>
+      <c r="G12" s="26">
+        <v>-1.81492795718315E-2</v>
+      </c>
+      <c r="H12" s="26">
+        <v>-6.7576209477786905E-2</v>
+      </c>
+      <c r="I12" s="26">
+        <v>0.84983064560491794</v>
+      </c>
+      <c r="J12" s="27">
+        <v>601.47640740497104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="33">
+        <f t="shared" si="0"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="B13" s="28">
+        <v>-3.2326958676074297E-2</v>
+      </c>
+      <c r="C13" s="28">
+        <v>-1.55532545623478</v>
+      </c>
+      <c r="D13" s="28">
+        <v>-0.40331732381847901</v>
+      </c>
+      <c r="E13" s="28">
+        <v>-9.3748180160615792E-3</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0.39112721806356598</v>
+      </c>
+      <c r="G13" s="28">
+        <v>-2.0165866190924E-2</v>
+      </c>
+      <c r="H13" s="28">
+        <v>-7.2581854624289496E-2</v>
+      </c>
+      <c r="I13" s="28">
+        <v>0.85483629075142098</v>
+      </c>
+      <c r="J13" s="29">
+        <v>668.30711933885505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="32">
+        <f t="shared" ref="A14:A23" si="1">A13+5%</f>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="B14" s="26">
+        <v>-3.55596545436817E-2</v>
+      </c>
+      <c r="C14" s="26">
+        <v>-1.71085800185825</v>
+      </c>
+      <c r="D14" s="26">
+        <v>-0.44364905620032702</v>
+      </c>
+      <c r="E14" s="26">
+        <v>-1.03122998176677E-2</v>
+      </c>
+      <c r="F14" s="26">
+        <v>0.43023993986992198</v>
+      </c>
+      <c r="G14" s="26">
+        <v>-2.2182452810016299E-2</v>
+      </c>
+      <c r="H14" s="26">
+        <v>-7.7264554922630901E-2</v>
+      </c>
+      <c r="I14" s="26">
+        <v>0.85951899104976204</v>
+      </c>
+      <c r="J14" s="27">
+        <v>735.13783127274303</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="33">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="B15" s="28">
+        <v>-3.87923504112892E-2</v>
+      </c>
+      <c r="C15" s="28">
+        <v>-1.8663905474817299</v>
+      </c>
+      <c r="D15" s="28">
+        <v>-0.48398078858217503</v>
+      </c>
+      <c r="E15" s="28">
+        <v>-1.12497816192739E-2</v>
+      </c>
+      <c r="F15" s="28">
+        <v>0.46935266167627898</v>
+      </c>
+      <c r="G15" s="28">
+        <v>-2.4199039429108699E-2</v>
+      </c>
+      <c r="H15" s="28">
+        <v>-8.1654586452325706E-2</v>
+      </c>
+      <c r="I15" s="28">
+        <v>0.86390902257945701</v>
+      </c>
+      <c r="J15" s="29">
+        <v>801.96854320662703</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="32">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="B16" s="26">
+        <v>-4.2025046278896597E-2</v>
+      </c>
+      <c r="C16" s="26">
+        <v>-2.0219230931052001</v>
+      </c>
+      <c r="D16" s="26">
+        <v>-0.52431252096402203</v>
+      </c>
+      <c r="E16" s="26">
+        <v>-1.218726342088E-2</v>
+      </c>
+      <c r="F16" s="26">
+        <v>0.50846538348263604</v>
+      </c>
+      <c r="G16" s="26">
+        <v>-2.6215626048201102E-2</v>
+      </c>
+      <c r="H16" s="26">
+        <v>-8.5778555465069406E-2</v>
+      </c>
+      <c r="I16" s="26">
+        <v>0.86803299159220104</v>
+      </c>
+      <c r="J16" s="27">
+        <v>868.79925514051297</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="33">
+        <f t="shared" si="1"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="B17" s="28">
+        <v>-4.5257742146504E-2</v>
+      </c>
+      <c r="C17" s="28">
+        <v>-2.1774556387286799</v>
+      </c>
+      <c r="D17" s="28">
+        <v>-0.56464425334586998</v>
+      </c>
+      <c r="E17" s="28">
+        <v>-1.31247452224862E-2</v>
+      </c>
+      <c r="F17" s="28">
+        <v>0.54757810528899198</v>
+      </c>
+      <c r="G17" s="28">
+        <v>-2.8232212667293501E-2</v>
+      </c>
+      <c r="H17" s="28">
+        <v>-8.9659938065298803E-2</v>
+      </c>
+      <c r="I17" s="28">
+        <v>0.87191437419242901</v>
+      </c>
+      <c r="J17" s="29">
+        <v>935.629967074398</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="32">
+        <f t="shared" si="1"/>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="B18" s="26">
+        <v>-4.84904380141115E-2</v>
+      </c>
+      <c r="C18" s="26">
+        <v>-2.33298818435216</v>
+      </c>
+      <c r="D18" s="26">
+        <v>-0.60497598572771905</v>
+      </c>
+      <c r="E18" s="26">
+        <v>-1.40622270240924E-2</v>
+      </c>
+      <c r="F18" s="26">
+        <v>0.58669082709534803</v>
+      </c>
+      <c r="G18" s="26">
+        <v>-3.0248799286385901E-2</v>
+      </c>
+      <c r="H18" s="26">
+        <v>-9.3319527374086497E-2</v>
+      </c>
+      <c r="I18" s="26">
+        <v>0.87557396350121797</v>
+      </c>
+      <c r="J18" s="27">
+        <v>1002.46067900828</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="33">
+        <f t="shared" si="1"/>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="B19" s="28">
+        <v>-5.1723133881718897E-2</v>
+      </c>
+      <c r="C19" s="28">
+        <v>-2.4885207299756398</v>
+      </c>
+      <c r="D19" s="28">
+        <v>-0.645307718109567</v>
+      </c>
+      <c r="E19" s="28">
+        <v>-1.49997088256985E-2</v>
+      </c>
+      <c r="F19" s="28">
+        <v>0.62580354890170498</v>
+      </c>
+      <c r="G19" s="28">
+        <v>-3.2265385905478297E-2</v>
+      </c>
+      <c r="H19" s="28">
+        <v>-9.6775806165719402E-2</v>
+      </c>
+      <c r="I19" s="28">
+        <v>0.87903024229285098</v>
+      </c>
+      <c r="J19" s="29">
+        <v>1069.29139094217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="32">
+        <f t="shared" si="1"/>
+        <v>0.8500000000000002</v>
+      </c>
+      <c r="B20" s="26">
+        <v>-5.49558297493263E-2</v>
+      </c>
+      <c r="C20" s="26">
+        <v>-2.6440532755991102</v>
+      </c>
+      <c r="D20" s="26">
+        <v>-0.68563945049141495</v>
+      </c>
+      <c r="E20" s="26">
+        <v>-1.5937190627304601E-2</v>
+      </c>
+      <c r="F20" s="26">
+        <v>0.66491627070806203</v>
+      </c>
+      <c r="G20" s="26">
+        <v>-3.42819725245707E-2</v>
+      </c>
+      <c r="H20" s="26">
+        <v>-0.100045259076723</v>
+      </c>
+      <c r="I20" s="26">
+        <v>0.88229969520385498</v>
+      </c>
+      <c r="J20" s="27">
+        <v>1136.1221028760599</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="33">
+        <f t="shared" si="1"/>
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="B21" s="28">
+        <v>-5.8188525616933703E-2</v>
+      </c>
+      <c r="C21" s="28">
+        <v>-2.7995858212226001</v>
+      </c>
+      <c r="D21" s="28">
+        <v>-0.72597118287326201</v>
+      </c>
+      <c r="E21" s="28">
+        <v>-1.68746724289108E-2</v>
+      </c>
+      <c r="F21" s="28">
+        <v>0.70402899251441797</v>
+      </c>
+      <c r="G21" s="28">
+        <v>-3.6298559143663103E-2</v>
+      </c>
+      <c r="H21" s="28">
+        <v>-0.103142635518727</v>
+      </c>
+      <c r="I21" s="28">
+        <v>0.88539707164585901</v>
+      </c>
+      <c r="J21" s="29">
+        <v>1202.95281480994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="32">
+        <f t="shared" si="1"/>
+        <v>0.95000000000000029</v>
+      </c>
+      <c r="B22" s="26">
+        <v>-6.14212214845411E-2</v>
+      </c>
+      <c r="C22" s="26">
+        <v>-2.9551183668460701</v>
+      </c>
+      <c r="D22" s="26">
+        <v>-0.76630291525511096</v>
+      </c>
+      <c r="E22" s="26">
+        <v>-1.7812154230517002E-2</v>
+      </c>
+      <c r="F22" s="26">
+        <v>0.74314171432077503</v>
+      </c>
+      <c r="G22" s="26">
+        <v>-3.8315145762755499E-2</v>
+      </c>
+      <c r="H22" s="26">
+        <v>-0.106081172143192</v>
+      </c>
+      <c r="I22" s="26">
+        <v>0.88833560827032299</v>
+      </c>
+      <c r="J22" s="27">
+        <v>1269.78352674383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="33">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="B23" s="28">
+        <v>-6.4653917352148593E-2</v>
+      </c>
+      <c r="C23" s="28">
+        <v>-3.1106509124695498</v>
+      </c>
+      <c r="D23" s="28">
+        <v>-0.80663464763695802</v>
+      </c>
+      <c r="E23" s="28">
+        <v>-1.8749636032123099E-2</v>
+      </c>
+      <c r="F23" s="28">
+        <v>0.78225443612713197</v>
+      </c>
+      <c r="G23" s="28">
+        <v>-4.0331732381847903E-2</v>
+      </c>
+      <c r="H23" s="28">
+        <v>-0.108872781936434</v>
+      </c>
+      <c r="I23" s="28">
+        <v>0.89112721806356598</v>
+      </c>
+      <c r="J23" s="29">
+        <v>1336.6142386777101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="1:10" ht="38.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="B29" s="26">
+        <v>-2.6011395387644701E-2</v>
+      </c>
+      <c r="C29" s="26">
+        <v>-0.236475523869839</v>
+      </c>
+      <c r="D29" s="26">
+        <v>-0.13105841239940499</v>
+      </c>
+      <c r="E29" s="26">
+        <v>-7.5433046624169796E-3</v>
+      </c>
+      <c r="F29" s="26">
+        <v>3.3446713329111297E-2</v>
+      </c>
+      <c r="G29" s="26">
+        <v>-6.5529206199701701E-3</v>
+      </c>
+      <c r="H29" s="26">
+        <v>-1.5765034924655901E-2</v>
+      </c>
+      <c r="I29" s="26">
+        <v>0.68469930150688196</v>
+      </c>
+      <c r="J29" s="27">
+        <v>45.785240594712398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="33">
+        <f>A29+5%</f>
+        <v>0.1</v>
+      </c>
+      <c r="B30" s="28">
+        <v>-5.2022790775289499E-2</v>
+      </c>
+      <c r="C30" s="28">
+        <v>-0.472951047739678</v>
+      </c>
+      <c r="D30" s="28">
+        <v>-0.26211682479880899</v>
+      </c>
+      <c r="E30" s="28">
+        <v>-1.5086609324834001E-2</v>
+      </c>
+      <c r="F30" s="28">
+        <v>6.6893426658222593E-2</v>
+      </c>
+      <c r="G30" s="28">
+        <v>-1.3105841239940399E-2</v>
+      </c>
+      <c r="H30" s="28">
+        <v>-3.0096884856161299E-2</v>
+      </c>
+      <c r="I30" s="28">
+        <v>0.69903115143838701</v>
+      </c>
+      <c r="J30" s="29">
+        <v>91.570481189424797</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="32">
+        <f t="shared" ref="A31:A48" si="2">A30+5%</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="B31" s="26">
+        <v>-7.8034186162934199E-2</v>
+      </c>
+      <c r="C31" s="26">
+        <v>-0.70942657160951705</v>
+      </c>
+      <c r="D31" s="26">
+        <v>-0.39317523719821301</v>
+      </c>
+      <c r="E31" s="26">
+        <v>-2.2629913987250901E-2</v>
+      </c>
+      <c r="F31" s="26">
+        <v>0.100340139987334</v>
+      </c>
+      <c r="G31" s="26">
+        <v>-1.9658761859910601E-2</v>
+      </c>
+      <c r="H31" s="26">
+        <v>-4.3182486967535898E-2</v>
+      </c>
+      <c r="I31" s="26">
+        <v>0.71211675354976001</v>
+      </c>
+      <c r="J31" s="27">
+        <v>137.35572178413801</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="33">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="B32" s="28">
+        <v>-0.104045581550579</v>
+      </c>
+      <c r="C32" s="28">
+        <v>-0.945902095479355</v>
+      </c>
+      <c r="D32" s="28">
+        <v>-0.52423364959761698</v>
+      </c>
+      <c r="E32" s="28">
+        <v>-3.0173218649667901E-2</v>
+      </c>
+      <c r="F32" s="28">
+        <v>0.13378685331644499</v>
+      </c>
+      <c r="G32" s="28">
+        <v>-2.6211682479880899E-2</v>
+      </c>
+      <c r="H32" s="28">
+        <v>-5.5177622236295798E-2</v>
+      </c>
+      <c r="I32" s="28">
+        <v>0.72411188881852095</v>
+      </c>
+      <c r="J32" s="29">
+        <v>183.14096237884999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="32">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="B33" s="26">
+        <v>-0.13005697693822399</v>
+      </c>
+      <c r="C33" s="26">
+        <v>-1.1823776193491999</v>
+      </c>
+      <c r="D33" s="26">
+        <v>-0.65529206199702195</v>
+      </c>
+      <c r="E33" s="26">
+        <v>-3.7716523312084999E-2</v>
+      </c>
+      <c r="F33" s="26">
+        <v>0.167233566645556</v>
+      </c>
+      <c r="G33" s="26">
+        <v>-3.2764603099851103E-2</v>
+      </c>
+      <c r="H33" s="26">
+        <v>-6.6213146683554894E-2</v>
+      </c>
+      <c r="I33" s="26">
+        <v>0.73514741326578104</v>
+      </c>
+      <c r="J33" s="27">
+        <v>228.926202973562</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="33">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="B34" s="28">
+        <v>-0.15606837232586901</v>
+      </c>
+      <c r="C34" s="28">
+        <v>-1.4188531432190301</v>
+      </c>
+      <c r="D34" s="28">
+        <v>-0.78635047439642602</v>
+      </c>
+      <c r="E34" s="28">
+        <v>-4.5259827974502002E-2</v>
+      </c>
+      <c r="F34" s="28">
+        <v>0.200680279974668</v>
+      </c>
+      <c r="G34" s="28">
+        <v>-3.93175237198213E-2</v>
+      </c>
+      <c r="H34" s="28">
+        <v>-7.6399784634871196E-2</v>
+      </c>
+      <c r="I34" s="28">
+        <v>0.74533405121709595</v>
+      </c>
+      <c r="J34" s="29">
+        <v>274.711443568275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="32">
+        <f t="shared" si="2"/>
+        <v>0.35</v>
+      </c>
+      <c r="B35" s="26">
+        <v>-0.182079767713513</v>
+      </c>
+      <c r="C35" s="26">
+        <v>-1.6553286670888701</v>
+      </c>
+      <c r="D35" s="26">
+        <v>-0.91740888679582999</v>
+      </c>
+      <c r="E35" s="26">
+        <v>-5.2803132636918902E-2</v>
+      </c>
+      <c r="F35" s="26">
+        <v>0.23412699330377901</v>
+      </c>
+      <c r="G35" s="26">
+        <v>-4.5870444339791497E-2</v>
+      </c>
+      <c r="H35" s="26">
+        <v>-8.5831856812015703E-2</v>
+      </c>
+      <c r="I35" s="26">
+        <v>0.75476612339424098</v>
+      </c>
+      <c r="J35" s="27">
+        <v>320.496684162988</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="33">
+        <f t="shared" si="2"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="B36" s="28">
+        <v>-0.20809116310115799</v>
+      </c>
+      <c r="C36" s="28">
+        <v>-1.89180419095871</v>
+      </c>
+      <c r="D36" s="28">
+        <v>-1.04846729919523</v>
+      </c>
+      <c r="E36" s="28">
+        <v>-6.0346437299335899E-2</v>
+      </c>
+      <c r="F36" s="28">
+        <v>0.26757370663288998</v>
+      </c>
+      <c r="G36" s="28">
+        <v>-5.2423364959761701E-2</v>
+      </c>
+      <c r="H36" s="28">
+        <v>-9.4590209547935705E-2</v>
+      </c>
+      <c r="I36" s="28">
+        <v>0.76352447613016095</v>
+      </c>
+      <c r="J36" s="29">
+        <v>366.28192475770101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="32">
+        <f t="shared" si="2"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="B37" s="26">
+        <v>-0.23410255848880299</v>
+      </c>
+      <c r="C37" s="26">
+        <v>-2.1282797148285502</v>
+      </c>
+      <c r="D37" s="26">
+        <v>-1.17952571159464</v>
+      </c>
+      <c r="E37" s="26">
+        <v>-6.7889741961752903E-2</v>
+      </c>
+      <c r="F37" s="26">
+        <v>0.30102041996200102</v>
+      </c>
+      <c r="G37" s="26">
+        <v>-5.8976285579731898E-2</v>
+      </c>
+      <c r="H37" s="26">
+        <v>-0.10274453795724001</v>
+      </c>
+      <c r="I37" s="26">
+        <v>0.77167880453946602</v>
+      </c>
+      <c r="J37" s="27">
+        <v>412.06716535241299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="33">
+        <f t="shared" si="2"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="B38" s="28">
+        <v>-0.26011395387644798</v>
+      </c>
+      <c r="C38" s="28">
+        <v>-2.3647552386983901</v>
+      </c>
+      <c r="D38" s="28">
+        <v>-1.3105841239940399</v>
+      </c>
+      <c r="E38" s="28">
+        <v>-7.5433046624169997E-2</v>
+      </c>
+      <c r="F38" s="28">
+        <v>0.33446713329111299</v>
+      </c>
+      <c r="G38" s="28">
+        <v>-6.5529206199702206E-2</v>
+      </c>
+      <c r="H38" s="28">
+        <v>-0.110355244472592</v>
+      </c>
+      <c r="I38" s="28">
+        <v>0.77928951105481703</v>
+      </c>
+      <c r="J38" s="29">
+        <v>457.852405947124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="32">
+        <f t="shared" si="2"/>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="B39" s="26">
+        <v>-0.286125349264093</v>
+      </c>
+      <c r="C39" s="26">
+        <v>-2.60123076256823</v>
+      </c>
+      <c r="D39" s="26">
+        <v>-1.44164253639345</v>
+      </c>
+      <c r="E39" s="26">
+        <v>-8.2976351286586897E-2</v>
+      </c>
+      <c r="F39" s="26">
+        <v>0.36791384662022403</v>
+      </c>
+      <c r="G39" s="26">
+        <v>-7.2082126819672396E-2</v>
+      </c>
+      <c r="H39" s="26">
+        <v>-0.117474937664372</v>
+      </c>
+      <c r="I39" s="26">
+        <v>0.78640920424659699</v>
+      </c>
+      <c r="J39" s="27">
+        <v>503.63764654183802</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="33">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="B40" s="28">
+        <v>-0.31213674465173702</v>
+      </c>
+      <c r="C40" s="28">
+        <v>-2.83770628643807</v>
+      </c>
+      <c r="D40" s="28">
+        <v>-1.5727009487928501</v>
+      </c>
+      <c r="E40" s="28">
+        <v>-9.0519655949003894E-2</v>
+      </c>
+      <c r="F40" s="28">
+        <v>0.40136055994933501</v>
+      </c>
+      <c r="G40" s="28">
+        <v>-7.86350474396426E-2</v>
+      </c>
+      <c r="H40" s="28">
+        <v>-0.124149650031666</v>
+      </c>
+      <c r="I40" s="28">
+        <v>0.79308391661389099</v>
+      </c>
+      <c r="J40" s="29">
+        <v>549.42288713655</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="32">
+        <f t="shared" si="2"/>
+        <v>0.65</v>
+      </c>
+      <c r="B41" s="26">
+        <v>-0.33814814003938198</v>
+      </c>
+      <c r="C41" s="26">
+        <v>-3.0741818103079099</v>
+      </c>
+      <c r="D41" s="26">
+        <v>-1.7037593611922599</v>
+      </c>
+      <c r="E41" s="26">
+        <v>-9.8062960611420794E-2</v>
+      </c>
+      <c r="F41" s="26">
+        <v>0.43480727327844598</v>
+      </c>
+      <c r="G41" s="26">
+        <v>-8.5187968059612804E-2</v>
+      </c>
+      <c r="H41" s="26">
+        <v>-0.13041983437669899</v>
+      </c>
+      <c r="I41" s="26">
+        <v>0.79935410095892501</v>
+      </c>
+      <c r="J41" s="27">
+        <v>595.20812773126295</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="33">
+        <f t="shared" si="2"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="B42" s="28">
+        <v>-0.364159535427027</v>
+      </c>
+      <c r="C42" s="28">
+        <v>-3.3106573341777499</v>
+      </c>
+      <c r="D42" s="28">
+        <v>-1.83481777359166</v>
+      </c>
+      <c r="E42" s="28">
+        <v>-0.105606265273838</v>
+      </c>
+      <c r="F42" s="28">
+        <v>0.46825398660755801</v>
+      </c>
+      <c r="G42" s="28">
+        <v>-9.1740888679582994E-2</v>
+      </c>
+      <c r="H42" s="28">
+        <v>-0.13632118434849599</v>
+      </c>
+      <c r="I42" s="28">
+        <v>0.80525545093072104</v>
+      </c>
+      <c r="J42" s="29">
+        <v>640.99336832597498</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="32">
+        <f t="shared" si="2"/>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="B43" s="26">
+        <v>-0.39017093081467202</v>
+      </c>
+      <c r="C43" s="26">
+        <v>-3.5471328580475898</v>
+      </c>
+      <c r="D43" s="26">
+        <v>-1.9658761859910701</v>
+      </c>
+      <c r="E43" s="26">
+        <v>-0.113149569936255</v>
+      </c>
+      <c r="F43" s="26">
+        <v>0.50170069993666899</v>
+      </c>
+      <c r="G43" s="26">
+        <v>-9.8293809299553198E-2</v>
+      </c>
+      <c r="H43" s="26">
+        <v>-0.14188531432190299</v>
+      </c>
+      <c r="I43" s="26">
+        <v>0.81081958090412898</v>
+      </c>
+      <c r="J43" s="27">
+        <v>686.778608920686</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="33">
+        <f t="shared" si="2"/>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="B44" s="28">
+        <v>-0.41618232620231699</v>
+      </c>
+      <c r="C44" s="28">
+        <v>-3.7836083819174302</v>
+      </c>
+      <c r="D44" s="28">
+        <v>-2.0969345983904701</v>
+      </c>
+      <c r="E44" s="28">
+        <v>-0.12069287459867201</v>
+      </c>
+      <c r="F44" s="28">
+        <v>0.53514741326577997</v>
+      </c>
+      <c r="G44" s="28">
+        <v>-0.104846729919523</v>
+      </c>
+      <c r="H44" s="28">
+        <v>-0.147140325963456</v>
+      </c>
+      <c r="I44" s="28">
+        <v>0.81607459254568104</v>
+      </c>
+      <c r="J44" s="29">
+        <v>732.56384951539997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="32">
+        <f t="shared" si="2"/>
+        <v>0.8500000000000002</v>
+      </c>
+      <c r="B45" s="26">
+        <v>-0.44219372158996101</v>
+      </c>
+      <c r="C45" s="26">
+        <v>-4.0200839057872599</v>
+      </c>
+      <c r="D45" s="26">
+        <v>-2.22799301078987</v>
+      </c>
+      <c r="E45" s="26">
+        <v>-0.12823617926108899</v>
+      </c>
+      <c r="F45" s="26">
+        <v>0.56859412659489195</v>
+      </c>
+      <c r="G45" s="26">
+        <v>-0.11139965053949399</v>
+      </c>
+      <c r="H45" s="26">
+        <v>-0.15211128292168</v>
+      </c>
+      <c r="I45" s="26">
+        <v>0.82104554950390596</v>
+      </c>
+      <c r="J45" s="27">
+        <v>778.34909011011302</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="33">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="B46" s="28">
+        <v>-0.46820511697760597</v>
+      </c>
+      <c r="C46" s="28">
+        <v>-4.2565594296571003</v>
+      </c>
+      <c r="D46" s="28">
+        <v>-2.3590514231892801</v>
+      </c>
+      <c r="E46" s="28">
+        <v>-0.135779483923506</v>
+      </c>
+      <c r="F46" s="28">
+        <v>0.60204083992400304</v>
+      </c>
+      <c r="G46" s="28">
+        <v>-0.117952571159464</v>
+      </c>
+      <c r="H46" s="28">
+        <v>-0.15682061056631399</v>
+      </c>
+      <c r="I46" s="28">
+        <v>0.82575487714854001</v>
+      </c>
+      <c r="J46" s="29">
+        <v>824.13433070482495</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="32">
+        <f t="shared" si="2"/>
+        <v>0.95000000000000029</v>
+      </c>
+      <c r="B47" s="26">
+        <v>-0.49421651236525099</v>
+      </c>
+      <c r="C47" s="26">
+        <v>-4.4930349535269398</v>
+      </c>
+      <c r="D47" s="26">
+        <v>-2.4901098355886799</v>
+      </c>
+      <c r="E47" s="26">
+        <v>-0.14332278858592301</v>
+      </c>
+      <c r="F47" s="26">
+        <v>0.63548755325311401</v>
+      </c>
+      <c r="G47" s="26">
+        <v>-0.124505491779434</v>
+      </c>
+      <c r="H47" s="26">
+        <v>-0.161288434229172</v>
+      </c>
+      <c r="I47" s="26">
+        <v>0.83022270081139804</v>
+      </c>
+      <c r="J47" s="27">
+        <v>869.91957129953698</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="33">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="B48" s="28">
+        <v>-0.52022790775289596</v>
+      </c>
+      <c r="C48" s="28">
+        <v>-4.7295104773967802</v>
+      </c>
+      <c r="D48" s="28">
+        <v>-2.62116824798809</v>
+      </c>
+      <c r="E48" s="28">
+        <v>-0.15086609324833999</v>
+      </c>
+      <c r="F48" s="28">
+        <v>0.66893426658222499</v>
+      </c>
+      <c r="G48" s="28">
+        <v>-0.131058412399404</v>
+      </c>
+      <c r="H48" s="28">
+        <v>-0.16553286670888701</v>
+      </c>
+      <c r="I48" s="28">
+        <v>0.83446713329111299</v>
+      </c>
+      <c r="J48" s="29">
+        <v>915.70481189424902</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+    </row>
+    <row r="52" spans="1:10" ht="38.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I52" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J52" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="B54" s="26">
+        <v>1.5198667779511101E-2</v>
+      </c>
+      <c r="C54" s="26">
+        <v>-0.10655422956924</v>
+      </c>
+      <c r="D54" s="26">
+        <v>3.5486408356591302E-2</v>
+      </c>
+      <c r="E54" s="26">
+        <v>4.4076136560581899E-3</v>
+      </c>
+      <c r="F54" s="26">
+        <v>4.2541203930153197E-2</v>
+      </c>
+      <c r="G54" s="26">
+        <v>1.7743204178295099E-3</v>
+      </c>
+      <c r="H54" s="26">
+        <v>-7.1036153046160101E-3</v>
+      </c>
+      <c r="I54" s="26">
+        <v>0.85792769390767998</v>
+      </c>
+      <c r="J54" s="27">
+        <v>101.611065078422</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="33">
+        <f>A54+5%</f>
+        <v>0.1</v>
+      </c>
+      <c r="B55" s="28">
+        <v>3.03973355590221E-2</v>
+      </c>
+      <c r="C55" s="28">
+        <v>-0.213108459138481</v>
+      </c>
+      <c r="D55" s="28">
+        <v>7.0972816713182604E-2</v>
+      </c>
+      <c r="E55" s="28">
+        <v>8.8152273121163797E-3</v>
+      </c>
+      <c r="F55" s="28">
+        <v>8.5082407860306394E-2</v>
+      </c>
+      <c r="G55" s="28">
+        <v>3.5486408356591001E-3</v>
+      </c>
+      <c r="H55" s="28">
+        <v>-1.35614473997215E-2</v>
+      </c>
+      <c r="I55" s="28">
+        <v>0.86438552600278595</v>
+      </c>
+      <c r="J55" s="29">
+        <v>203.222130156845</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="32">
+        <f t="shared" ref="A56:A73" si="3">A55+5%</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="B56" s="26">
+        <v>4.5596003338533198E-2</v>
+      </c>
+      <c r="C56" s="26">
+        <v>-0.31966268870772102</v>
+      </c>
+      <c r="D56" s="26">
+        <v>0.106459225069774</v>
+      </c>
+      <c r="E56" s="26">
+        <v>1.3222840968174601E-2</v>
+      </c>
+      <c r="F56" s="26">
+        <v>0.127623611790459</v>
+      </c>
+      <c r="G56" s="26">
+        <v>5.3229612534886903E-3</v>
+      </c>
+      <c r="H56" s="26">
+        <v>-1.9457728877861302E-2</v>
+      </c>
+      <c r="I56" s="26">
+        <v>0.87028180748092399</v>
+      </c>
+      <c r="J56" s="27">
+        <v>304.83319523526802</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="33">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="B57" s="28">
+        <v>6.0794671118044201E-2</v>
+      </c>
+      <c r="C57" s="28">
+        <v>-0.42621691827696101</v>
+      </c>
+      <c r="D57" s="28">
+        <v>0.14194563342636499</v>
+      </c>
+      <c r="E57" s="28">
+        <v>1.7630454624232801E-2</v>
+      </c>
+      <c r="F57" s="28">
+        <v>0.17016481572061301</v>
+      </c>
+      <c r="G57" s="28">
+        <v>7.09728167131828E-3</v>
+      </c>
+      <c r="H57" s="28">
+        <v>-2.48626535661561E-2</v>
+      </c>
+      <c r="I57" s="28">
+        <v>0.875686732169219</v>
+      </c>
+      <c r="J57" s="29">
+        <v>406.44426031368999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="32">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="B58" s="26">
+        <v>7.5993338897555301E-2</v>
+      </c>
+      <c r="C58" s="26">
+        <v>-0.53277114784620205</v>
+      </c>
+      <c r="D58" s="26">
+        <v>0.17743204178295699</v>
+      </c>
+      <c r="E58" s="26">
+        <v>2.2038068280291E-2</v>
+      </c>
+      <c r="F58" s="26">
+        <v>0.21270601965076599</v>
+      </c>
+      <c r="G58" s="26">
+        <v>8.8716020891478706E-3</v>
+      </c>
+      <c r="H58" s="26">
+        <v>-2.9835184279387202E-2</v>
+      </c>
+      <c r="I58" s="26">
+        <v>0.880659262882451</v>
+      </c>
+      <c r="J58" s="27">
+        <v>508.05532539211202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="33">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="B59" s="28">
+        <v>9.1192006677066395E-2</v>
+      </c>
+      <c r="C59" s="28">
+        <v>-0.63932537741544204</v>
+      </c>
+      <c r="D59" s="28">
+        <v>0.21291845013954799</v>
+      </c>
+      <c r="E59" s="28">
+        <v>2.6445681936349202E-2</v>
+      </c>
+      <c r="F59" s="28">
+        <v>0.255247223580919</v>
+      </c>
+      <c r="G59" s="28">
+        <v>1.06459225069774E-2</v>
+      </c>
+      <c r="H59" s="28">
+        <v>-3.4425212630062298E-2</v>
+      </c>
+      <c r="I59" s="28">
+        <v>0.88524929123312601</v>
+      </c>
+      <c r="J59" s="29">
+        <v>609.66639047053604</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="32">
+        <f t="shared" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="B60" s="26">
+        <v>0.106390674456578</v>
+      </c>
+      <c r="C60" s="26">
+        <v>-0.74587960698468203</v>
+      </c>
+      <c r="D60" s="26">
+        <v>0.248404858496139</v>
+      </c>
+      <c r="E60" s="26">
+        <v>3.0853295592407501E-2</v>
+      </c>
+      <c r="F60" s="26">
+        <v>0.29778842751107198</v>
+      </c>
+      <c r="G60" s="26">
+        <v>1.2420242924807E-2</v>
+      </c>
+      <c r="H60" s="26">
+        <v>-3.8675238880687302E-2</v>
+      </c>
+      <c r="I60" s="26">
+        <v>0.889499317483751</v>
+      </c>
+      <c r="J60" s="27">
+        <v>711.27745554895796</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="33">
+        <f t="shared" si="3"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="B61" s="28">
+        <v>0.121589342236089</v>
+      </c>
+      <c r="C61" s="28">
+        <v>-0.85243383655392202</v>
+      </c>
+      <c r="D61" s="28">
+        <v>0.28389126685273097</v>
+      </c>
+      <c r="E61" s="28">
+        <v>3.5260909248465602E-2</v>
+      </c>
+      <c r="F61" s="28">
+        <v>0.34032963144122502</v>
+      </c>
+      <c r="G61" s="28">
+        <v>1.41945633426366E-2</v>
+      </c>
+      <c r="H61" s="28">
+        <v>-4.26216918276962E-2</v>
+      </c>
+      <c r="I61" s="28">
+        <v>0.89344577043076001</v>
+      </c>
+      <c r="J61" s="29">
+        <v>812.88852062738101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="32">
+        <f t="shared" si="3"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="B62" s="26">
+        <v>0.13678801001560001</v>
+      </c>
+      <c r="C62" s="26">
+        <v>-0.95898806612316301</v>
+      </c>
+      <c r="D62" s="26">
+        <v>0.31937767520932198</v>
+      </c>
+      <c r="E62" s="26">
+        <v>3.9668522904523801E-2</v>
+      </c>
+      <c r="F62" s="26">
+        <v>0.382870835371378</v>
+      </c>
+      <c r="G62" s="26">
+        <v>1.59688837604661E-2</v>
+      </c>
+      <c r="H62" s="26">
+        <v>-4.6295975605945901E-2</v>
+      </c>
+      <c r="I62" s="26">
+        <v>0.89712005420900898</v>
+      </c>
+      <c r="J62" s="27">
+        <v>914.49958570580304</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="33">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="B63" s="28">
+        <v>0.15198667779511099</v>
+      </c>
+      <c r="C63" s="28">
+        <v>-1.0655422956924001</v>
+      </c>
+      <c r="D63" s="28">
+        <v>0.35486408356591298</v>
+      </c>
+      <c r="E63" s="28">
+        <v>4.4076136560582201E-2</v>
+      </c>
+      <c r="F63" s="28">
+        <v>0.42541203930153199</v>
+      </c>
+      <c r="G63" s="28">
+        <v>1.77432041782957E-2</v>
+      </c>
+      <c r="H63" s="28">
+        <v>-4.9725307132311998E-2</v>
+      </c>
+      <c r="I63" s="28">
+        <v>0.90054938573537602</v>
+      </c>
+      <c r="J63" s="29">
+        <v>1016.11065078423</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="32">
+        <f t="shared" si="3"/>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="B64" s="26">
+        <v>0.167185345574622</v>
+      </c>
+      <c r="C64" s="26">
+        <v>-1.17209652526164</v>
+      </c>
+      <c r="D64" s="26">
+        <v>0.39035049192250498</v>
+      </c>
+      <c r="E64" s="26">
+        <v>4.8483750216640302E-2</v>
+      </c>
+      <c r="F64" s="26">
+        <v>0.46795324323168502</v>
+      </c>
+      <c r="G64" s="26">
+        <v>1.95175245961253E-2</v>
+      </c>
+      <c r="H64" s="26">
+        <v>-5.2933391463429097E-2</v>
+      </c>
+      <c r="I64" s="26">
+        <v>0.90375747006649298</v>
+      </c>
+      <c r="J64" s="27">
+        <v>1117.7217158626499</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="33">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="B65" s="28">
+        <v>0.18238401335413301</v>
+      </c>
+      <c r="C65" s="28">
+        <v>-1.2786507548308801</v>
+      </c>
+      <c r="D65" s="28">
+        <v>0.42583690027909599</v>
+      </c>
+      <c r="E65" s="28">
+        <v>5.2891363872698403E-2</v>
+      </c>
+      <c r="F65" s="28">
+        <v>0.51049444716183801</v>
+      </c>
+      <c r="G65" s="28">
+        <v>2.1291845013954799E-2</v>
+      </c>
+      <c r="H65" s="28">
+        <v>-5.5940970523851198E-2</v>
+      </c>
+      <c r="I65" s="28">
+        <v>0.90676504912691502</v>
+      </c>
+      <c r="J65" s="29">
+        <v>1219.33278094107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="32">
+        <f t="shared" si="3"/>
+        <v>0.65</v>
+      </c>
+      <c r="B66" s="26">
+        <v>0.19758268113364399</v>
+      </c>
+      <c r="C66" s="26">
+        <v>-1.38520498440012</v>
+      </c>
+      <c r="D66" s="26">
+        <v>0.46132330863568699</v>
+      </c>
+      <c r="E66" s="26">
+        <v>5.7298977528756699E-2</v>
+      </c>
+      <c r="F66" s="26">
+        <v>0.55303565109199104</v>
+      </c>
+      <c r="G66" s="26">
+        <v>2.3066165431784399E-2</v>
+      </c>
+      <c r="H66" s="26">
+        <v>-5.8766272065459799E-2</v>
+      </c>
+      <c r="I66" s="26">
+        <v>0.90959035066852301</v>
+      </c>
+      <c r="J66" s="27">
+        <v>1320.9438460194899</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="33">
+        <f t="shared" si="3"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="B67" s="28">
+        <v>0.21278134891315501</v>
+      </c>
+      <c r="C67" s="28">
+        <v>-1.4917592139693601</v>
+      </c>
+      <c r="D67" s="28">
+        <v>0.49680971699227899</v>
+      </c>
+      <c r="E67" s="28">
+        <v>6.1706591184814898E-2</v>
+      </c>
+      <c r="F67" s="28">
+        <v>0.59557685502214397</v>
+      </c>
+      <c r="G67" s="28">
+        <v>2.4840485849614E-2</v>
+      </c>
+      <c r="H67" s="28">
+        <v>-6.1425379398738503E-2</v>
+      </c>
+      <c r="I67" s="28">
+        <v>0.91224945800180202</v>
+      </c>
+      <c r="J67" s="29">
+        <v>1422.55491109792</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="32">
+        <f t="shared" si="3"/>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="B68" s="26">
+        <v>0.22798001669266599</v>
+      </c>
+      <c r="C68" s="26">
+        <v>-1.5983134435386099</v>
+      </c>
+      <c r="D68" s="26">
+        <v>0.53229612534887005</v>
+      </c>
+      <c r="E68" s="26">
+        <v>6.6114204840873103E-2</v>
+      </c>
+      <c r="F68" s="26">
+        <v>0.63811805895229801</v>
+      </c>
+      <c r="G68" s="26">
+        <v>2.6614806267443499E-2</v>
+      </c>
+      <c r="H68" s="26">
+        <v>-6.3932537741544102E-2</v>
+      </c>
+      <c r="I68" s="26">
+        <v>0.91475661634460803</v>
+      </c>
+      <c r="J68" s="27">
+        <v>1524.1659761763401</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="33">
+        <f t="shared" si="3"/>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="B69" s="28">
+        <v>0.243178684472177</v>
+      </c>
+      <c r="C69" s="28">
+        <v>-1.70486767310785</v>
+      </c>
+      <c r="D69" s="28">
+        <v>0.56778253370546095</v>
+      </c>
+      <c r="E69" s="28">
+        <v>7.0521818496931302E-2</v>
+      </c>
+      <c r="F69" s="28">
+        <v>0.68065926288245104</v>
+      </c>
+      <c r="G69" s="28">
+        <v>2.8389126685273099E-2</v>
+      </c>
+      <c r="H69" s="28">
+        <v>-6.6300409509749594E-2</v>
+      </c>
+      <c r="I69" s="28">
+        <v>0.917124488112813</v>
+      </c>
+      <c r="J69" s="29">
+        <v>1625.77704125476</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="32">
+        <f t="shared" si="3"/>
+        <v>0.8500000000000002</v>
+      </c>
+      <c r="B70" s="26">
+        <v>0.25837735225168801</v>
+      </c>
+      <c r="C70" s="26">
+        <v>-1.8114219026770899</v>
+      </c>
+      <c r="D70" s="26">
+        <v>0.60326894206205295</v>
+      </c>
+      <c r="E70" s="26">
+        <v>7.4929432152989597E-2</v>
+      </c>
+      <c r="F70" s="26">
+        <v>0.72320046681260397</v>
+      </c>
+      <c r="G70" s="26">
+        <v>3.0163447103102599E-2</v>
+      </c>
+      <c r="H70" s="26">
+        <v>-6.8540288209403305E-2</v>
+      </c>
+      <c r="I70" s="26">
+        <v>0.91936436681246703</v>
+      </c>
+      <c r="J70" s="27">
+        <v>1727.3881063331801</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="33">
+        <f t="shared" si="3"/>
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="B71" s="28">
+        <v>0.27357602003119902</v>
+      </c>
+      <c r="C71" s="28">
+        <v>-1.91797613224633</v>
+      </c>
+      <c r="D71" s="28">
+        <v>0.63875535041864395</v>
+      </c>
+      <c r="E71" s="28">
+        <v>7.9337045809047796E-2</v>
+      </c>
+      <c r="F71" s="28">
+        <v>0.76574167074275701</v>
+      </c>
+      <c r="G71" s="28">
+        <v>3.1937767520932199E-2</v>
+      </c>
+      <c r="H71" s="28">
+        <v>-7.0662278556443595E-2</v>
+      </c>
+      <c r="I71" s="28">
+        <v>0.921486357159507</v>
+      </c>
+      <c r="J71" s="29">
+        <v>1828.99917141161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="32">
+        <f t="shared" si="3"/>
+        <v>0.95000000000000029</v>
+      </c>
+      <c r="B72" s="26">
+        <v>0.28877468781070997</v>
+      </c>
+      <c r="C72" s="26">
+        <v>-2.0245303618155699</v>
+      </c>
+      <c r="D72" s="26">
+        <v>0.67424175877523496</v>
+      </c>
+      <c r="E72" s="26">
+        <v>8.3744659465105897E-2</v>
+      </c>
+      <c r="F72" s="26">
+        <v>0.80828287467291005</v>
+      </c>
+      <c r="G72" s="26">
+        <v>3.3712087938761799E-2</v>
+      </c>
+      <c r="H72" s="26">
+        <v>-7.2675448885687E-2</v>
+      </c>
+      <c r="I72" s="26">
+        <v>0.92349952748875097</v>
+      </c>
+      <c r="J72" s="27">
+        <v>1930.61023649003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="33">
+        <f t="shared" si="3"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="B73" s="28">
+        <v>0.30397335559022098</v>
+      </c>
+      <c r="C73" s="28">
+        <v>-2.13108459138481</v>
+      </c>
+      <c r="D73" s="28">
+        <v>0.70972816713182696</v>
+      </c>
+      <c r="E73" s="28">
+        <v>8.8152273121163999E-2</v>
+      </c>
+      <c r="F73" s="28">
+        <v>0.85082407860306397</v>
+      </c>
+      <c r="G73" s="28">
+        <v>3.5486408356591302E-2</v>
+      </c>
+      <c r="H73" s="28">
+        <v>-7.4587960698468195E-2</v>
+      </c>
+      <c r="I73" s="28">
+        <v>0.92541203930153204</v>
+      </c>
+      <c r="J73" s="29">
+        <v>2032.2213015684499</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A51:J51"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="7" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="10" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="B4" s="26">
+        <v>-6.0201044544565901E-2</v>
+      </c>
+      <c r="C4" s="26">
+        <v>-7.03171225018954E-3</v>
+      </c>
+      <c r="D4" s="26">
+        <v>-7.9992314157480995E-2</v>
+      </c>
+      <c r="E4" s="26">
+        <v>3.2541697082075799E-2</v>
+      </c>
+      <c r="F4" s="26">
+        <v>-4.9221985751325703E-4</v>
+      </c>
+      <c r="G4" s="26">
+        <v>-3.9996157078740499E-3</v>
+      </c>
+      <c r="H4" s="26">
+        <v>-1.6626955159927799E-2</v>
+      </c>
+      <c r="I4" s="26">
+        <v>0.66746089680144405</v>
+      </c>
+      <c r="J4" s="27">
+        <v>702776.37507396005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
+        <f>A4+5%</f>
+        <v>0.1</v>
+      </c>
+      <c r="B5" s="28">
+        <v>-0.120402089089132</v>
+      </c>
+      <c r="C5" s="28">
+        <v>-1.40634245003778E-2</v>
+      </c>
+      <c r="D5" s="28">
+        <v>-0.15998462831496199</v>
+      </c>
+      <c r="E5" s="28">
+        <v>6.5083394164151806E-2</v>
+      </c>
+      <c r="F5" s="28">
+        <v>-9.8443971502643296E-4</v>
+      </c>
+      <c r="G5" s="28">
+        <v>-7.9992314157481207E-3</v>
+      </c>
+      <c r="H5" s="28">
+        <v>-3.1742368941680303E-2</v>
+      </c>
+      <c r="I5" s="28">
+        <v>0.68257631058319801</v>
+      </c>
+      <c r="J5" s="29">
+        <v>1405552.7501479201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <f t="shared" ref="A6:A23" si="0">A5+5%</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="B6" s="26">
+        <v>-0.18060313363369801</v>
+      </c>
+      <c r="C6" s="26">
+        <v>-2.1095136750566498E-2</v>
+      </c>
+      <c r="D6" s="26">
+        <v>-0.239976942472443</v>
+      </c>
+      <c r="E6" s="26">
+        <v>9.7625091246227605E-2</v>
+      </c>
+      <c r="F6" s="26">
+        <v>-1.47665957253964E-3</v>
+      </c>
+      <c r="G6" s="26">
+        <v>-1.1998847123622199E-2</v>
+      </c>
+      <c r="H6" s="26">
+        <v>-4.55433989163238E-2</v>
+      </c>
+      <c r="I6" s="26">
+        <v>0.69637734055783995</v>
+      </c>
+      <c r="J6" s="27">
+        <v>2108329.1252218699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="B7" s="28">
+        <v>-0.24080417817826399</v>
+      </c>
+      <c r="C7" s="28">
+        <v>-2.81268490007552E-2</v>
+      </c>
+      <c r="D7" s="28">
+        <v>-0.31996925662992398</v>
+      </c>
+      <c r="E7" s="28">
+        <v>0.130166788328303</v>
+      </c>
+      <c r="F7" s="28">
+        <v>-1.9688794300528499E-3</v>
+      </c>
+      <c r="G7" s="28">
+        <v>-1.59984628314962E-2</v>
+      </c>
+      <c r="H7" s="28">
+        <v>-5.8194343059747203E-2</v>
+      </c>
+      <c r="I7" s="28">
+        <v>0.709028284701264</v>
+      </c>
+      <c r="J7" s="29">
+        <v>2811105.50029583</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="B8" s="26">
+        <v>-0.30100522272282998</v>
+      </c>
+      <c r="C8" s="26">
+        <v>-3.5158561250944499E-2</v>
+      </c>
+      <c r="D8" s="26">
+        <v>-0.39996157078740502</v>
+      </c>
+      <c r="E8" s="26">
+        <v>0.16270848541037899</v>
+      </c>
+      <c r="F8" s="26">
+        <v>-2.4610992875661098E-3</v>
+      </c>
+      <c r="G8" s="26">
+        <v>-1.9998078539370301E-2</v>
+      </c>
+      <c r="H8" s="26">
+        <v>-6.9833211671696496E-2</v>
+      </c>
+      <c r="I8" s="26">
+        <v>0.72066715331321296</v>
+      </c>
+      <c r="J8" s="27">
+        <v>3513881.87536979</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="B9" s="28">
+        <v>-0.36120626726739602</v>
+      </c>
+      <c r="C9" s="28">
+        <v>-4.2190273501133101E-2</v>
+      </c>
+      <c r="D9" s="28">
+        <v>-0.479953884944887</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0.19525018249245499</v>
+      </c>
+      <c r="F9" s="28">
+        <v>-2.9533191450793E-3</v>
+      </c>
+      <c r="G9" s="28">
+        <v>-2.3997694247244301E-2</v>
+      </c>
+      <c r="H9" s="28">
+        <v>-8.0576782698111402E-2</v>
+      </c>
+      <c r="I9" s="28">
+        <v>0.73141072433962895</v>
+      </c>
+      <c r="J9" s="29">
+        <v>4216658.2504437501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="32">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="B10" s="26">
+        <v>-0.421407311811962</v>
+      </c>
+      <c r="C10" s="26">
+        <v>-4.9221985751322E-2</v>
+      </c>
+      <c r="D10" s="26">
+        <v>-0.55994619910236698</v>
+      </c>
+      <c r="E10" s="26">
+        <v>0.22779187957453101</v>
+      </c>
+      <c r="F10" s="26">
+        <v>-3.44553900259252E-3</v>
+      </c>
+      <c r="G10" s="26">
+        <v>-2.7997309955118399E-2</v>
+      </c>
+      <c r="H10" s="26">
+        <v>-9.0524533648495498E-2</v>
+      </c>
+      <c r="I10" s="26">
+        <v>0.74135847529001198</v>
+      </c>
+      <c r="J10" s="27">
+        <v>4919434.6255176999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="B11" s="28">
+        <v>-0.48160835635652699</v>
+      </c>
+      <c r="C11" s="28">
+        <v>-5.6253698001510699E-2</v>
+      </c>
+      <c r="D11" s="28">
+        <v>-0.63993851325984896</v>
+      </c>
+      <c r="E11" s="28">
+        <v>0.260333576656607</v>
+      </c>
+      <c r="F11" s="28">
+        <v>-3.9377588601057396E-3</v>
+      </c>
+      <c r="G11" s="28">
+        <v>-3.19969256629924E-2</v>
+      </c>
+      <c r="H11" s="28">
+        <v>-9.9761730959566405E-2</v>
+      </c>
+      <c r="I11" s="28">
+        <v>0.75059567260108395</v>
+      </c>
+      <c r="J11" s="29">
+        <v>5622211.0005916702</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="B12" s="26">
+        <v>-0.54180940090109297</v>
+      </c>
+      <c r="C12" s="26">
+        <v>-6.3285410251699398E-2</v>
+      </c>
+      <c r="D12" s="26">
+        <v>-0.71993082741732894</v>
+      </c>
+      <c r="E12" s="26">
+        <v>0.292875273738683</v>
+      </c>
+      <c r="F12" s="26">
+        <v>-4.4299787176189497E-3</v>
+      </c>
+      <c r="G12" s="26">
+        <v>-3.5996541370866497E-2</v>
+      </c>
+      <c r="H12" s="26">
+        <v>-0.108361880180219</v>
+      </c>
+      <c r="I12" s="26">
+        <v>0.75919582182173595</v>
+      </c>
+      <c r="J12" s="27">
+        <v>6324987.3756656302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="33">
+        <f t="shared" si="0"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="B13" s="28">
+        <v>-0.60201044544565896</v>
+      </c>
+      <c r="C13" s="28">
+        <v>-7.0317122501888402E-2</v>
+      </c>
+      <c r="D13" s="28">
+        <v>-0.79992314157481004</v>
+      </c>
+      <c r="E13" s="28">
+        <v>0.32541697082075899</v>
+      </c>
+      <c r="F13" s="28">
+        <v>-4.9221985751321798E-3</v>
+      </c>
+      <c r="G13" s="28">
+        <v>-3.9996157078740498E-2</v>
+      </c>
+      <c r="H13" s="28">
+        <v>-0.116388686119494</v>
+      </c>
+      <c r="I13" s="28">
+        <v>0.76722262776101202</v>
+      </c>
+      <c r="J13" s="29">
+        <v>7027763.7507395903</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="32">
+        <f t="shared" si="0"/>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="B14" s="26">
+        <v>-0.66221148999022506</v>
+      </c>
+      <c r="C14" s="26">
+        <v>-7.7348834752077406E-2</v>
+      </c>
+      <c r="D14" s="26">
+        <v>-0.87991545573229302</v>
+      </c>
+      <c r="E14" s="26">
+        <v>0.35795866790283398</v>
+      </c>
+      <c r="F14" s="26">
+        <v>-5.4144184326454002E-3</v>
+      </c>
+      <c r="G14" s="26">
+        <v>-4.3995772786614602E-2</v>
+      </c>
+      <c r="H14" s="26">
+        <v>-0.123897633611075</v>
+      </c>
+      <c r="I14" s="26">
+        <v>0.77473157525259195</v>
+      </c>
+      <c r="J14" s="27">
+        <v>7730540.1258135503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="33">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="B15" s="28">
+        <v>-0.72241253453479204</v>
+      </c>
+      <c r="C15" s="28">
+        <v>-8.4380547002266298E-2</v>
+      </c>
+      <c r="D15" s="28">
+        <v>-0.959907769889773</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0.39050036498491097</v>
+      </c>
+      <c r="F15" s="28">
+        <v>-5.9066382901586199E-3</v>
+      </c>
+      <c r="G15" s="28">
+        <v>-4.79953884944887E-2</v>
+      </c>
+      <c r="H15" s="28">
+        <v>-0.13093727188443099</v>
+      </c>
+      <c r="I15" s="28">
+        <v>0.78177121352594903</v>
+      </c>
+      <c r="J15" s="29">
+        <v>8433316.5008875001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="32">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="B16" s="26">
+        <v>-0.78261357907935702</v>
+      </c>
+      <c r="C16" s="26">
+        <v>-9.1412259252455094E-2</v>
+      </c>
+      <c r="D16" s="26">
+        <v>-1.0399000840472501</v>
+      </c>
+      <c r="E16" s="26">
+        <v>0.42304206206698602</v>
+      </c>
+      <c r="F16" s="26">
+        <v>-6.3988581476718499E-3</v>
+      </c>
+      <c r="G16" s="26">
+        <v>-5.19950042023627E-2</v>
+      </c>
+      <c r="H16" s="26">
+        <v>-0.13755026541394799</v>
+      </c>
+      <c r="I16" s="26">
+        <v>0.78838420705546497</v>
+      </c>
+      <c r="J16" s="27">
+        <v>9136092.8759614602</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="33">
+        <f t="shared" si="0"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="B17" s="28">
+        <v>-0.84281462362392401</v>
+      </c>
+      <c r="C17" s="28">
+        <v>-9.8443971502643599E-2</v>
+      </c>
+      <c r="D17" s="28">
+        <v>-1.11989239820473</v>
+      </c>
+      <c r="E17" s="28">
+        <v>0.45558375914906202</v>
+      </c>
+      <c r="F17" s="28">
+        <v>-6.89107800518504E-3</v>
+      </c>
+      <c r="G17" s="28">
+        <v>-5.5994619910236798E-2</v>
+      </c>
+      <c r="H17" s="28">
+        <v>-0.143774259324081</v>
+      </c>
+      <c r="I17" s="28">
+        <v>0.79460820096559903</v>
+      </c>
+      <c r="J17" s="29">
+        <v>9838869.2510353997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="32">
+        <f t="shared" si="0"/>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="B18" s="26">
+        <v>-0.90301566816848999</v>
+      </c>
+      <c r="C18" s="26">
+        <v>-0.105475683752833</v>
+      </c>
+      <c r="D18" s="26">
+        <v>-1.1998847123622201</v>
+      </c>
+      <c r="E18" s="26">
+        <v>0.48812545623113801</v>
+      </c>
+      <c r="F18" s="26">
+        <v>-7.3832978626982796E-3</v>
+      </c>
+      <c r="G18" s="26">
+        <v>-5.9994235618110799E-2</v>
+      </c>
+      <c r="H18" s="26">
+        <v>-0.14964259643934999</v>
+      </c>
+      <c r="I18" s="26">
+        <v>0.80047653808086705</v>
+      </c>
+      <c r="J18" s="27">
+        <v>10541645.626109401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="33">
+        <f t="shared" si="0"/>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="B19" s="28">
+        <v>-0.96321671271305498</v>
+      </c>
+      <c r="C19" s="28">
+        <v>-0.11250739600302199</v>
+      </c>
+      <c r="D19" s="28">
+        <v>-1.2798770265196999</v>
+      </c>
+      <c r="E19" s="28">
+        <v>0.520667153313214</v>
+      </c>
+      <c r="F19" s="28">
+        <v>-7.8755177202115001E-3</v>
+      </c>
+      <c r="G19" s="28">
+        <v>-6.3993851325984799E-2</v>
+      </c>
+      <c r="H19" s="28">
+        <v>-0.155184914825992</v>
+      </c>
+      <c r="I19" s="28">
+        <v>0.80601885646750904</v>
+      </c>
+      <c r="J19" s="29">
+        <v>11244422.001183299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="32">
+        <f t="shared" si="0"/>
+        <v>0.8500000000000002</v>
+      </c>
+      <c r="B20" s="26">
+        <v>-1.02341775725762</v>
+      </c>
+      <c r="C20" s="26">
+        <v>-0.11953910825321</v>
+      </c>
+      <c r="D20" s="26">
+        <v>-1.35986934067718</v>
+      </c>
+      <c r="E20" s="26">
+        <v>0.55320885039529</v>
+      </c>
+      <c r="F20" s="26">
+        <v>-8.3677375777246894E-3</v>
+      </c>
+      <c r="G20" s="26">
+        <v>-6.7993467033859001E-2</v>
+      </c>
+      <c r="H20" s="26">
+        <v>-0.160427648434979</v>
+      </c>
+      <c r="I20" s="26">
+        <v>0.81126159007649601</v>
+      </c>
+      <c r="J20" s="27">
+        <v>11947198.3762573</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="33">
+        <f t="shared" si="0"/>
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="B21" s="28">
+        <v>-1.0836188018021899</v>
+      </c>
+      <c r="C21" s="28">
+        <v>-0.12657082050339899</v>
+      </c>
+      <c r="D21" s="28">
+        <v>-1.4398616548346601</v>
+      </c>
+      <c r="E21" s="28">
+        <v>0.58575054747736499</v>
+      </c>
+      <c r="F21" s="28">
+        <v>-8.8599574352379307E-3</v>
+      </c>
+      <c r="G21" s="28">
+        <v>-7.1993082741732994E-2</v>
+      </c>
+      <c r="H21" s="28">
+        <v>-0.16539444869612299</v>
+      </c>
+      <c r="I21" s="28">
+        <v>0.81622839033764105</v>
+      </c>
+      <c r="J21" s="29">
+        <v>12649974.7513313</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.95000000000000029</v>
+      </c>
+      <c r="B22" s="26">
+        <v>-1.1438198463467499</v>
+      </c>
+      <c r="C22" s="26">
+        <v>-0.13360253275358799</v>
+      </c>
+      <c r="D22" s="26">
+        <v>-1.51985396899214</v>
+      </c>
+      <c r="E22" s="26">
+        <v>0.61829224455944098</v>
+      </c>
+      <c r="F22" s="26">
+        <v>-9.3521772927511407E-3</v>
+      </c>
+      <c r="G22" s="26">
+        <v>-7.5992698449607002E-2</v>
+      </c>
+      <c r="H22" s="26">
+        <v>-0.17010654125156899</v>
+      </c>
+      <c r="I22" s="26">
+        <v>0.82094048289308497</v>
+      </c>
+      <c r="J22" s="27">
+        <v>13352751.1264052</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="33">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="B23" s="28">
+        <v>-1.2040208908913199</v>
+      </c>
+      <c r="C23" s="28">
+        <v>-0.140634245003777</v>
+      </c>
+      <c r="D23" s="28">
+        <v>-1.5998462831496201</v>
+      </c>
+      <c r="E23" s="28">
+        <v>0.65083394164151698</v>
+      </c>
+      <c r="F23" s="28">
+        <v>-9.8443971502643699E-3</v>
+      </c>
+      <c r="G23" s="28">
+        <v>-7.9992314157481106E-2</v>
+      </c>
+      <c r="H23" s="28">
+        <v>-0.17458302917924101</v>
+      </c>
+      <c r="I23" s="28">
+        <v>0.82541697082075804</v>
+      </c>
+      <c r="J23" s="29">
+        <v>14055527.501479199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="1:10" ht="38.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="B29" s="26">
+        <v>-7.1396951464903005E-2</v>
+      </c>
+      <c r="C29" s="26">
+        <v>-4.04299270187162E-2</v>
+      </c>
+      <c r="D29" s="26">
+        <v>-0.14225526564209501</v>
+      </c>
+      <c r="E29" s="26">
+        <v>2.92948840751781E-2</v>
+      </c>
+      <c r="F29" s="26">
+        <v>-2.8300948913101199E-3</v>
+      </c>
+      <c r="G29" s="26">
+        <v>-7.1127632821047998E-3</v>
+      </c>
+      <c r="H29" s="26">
+        <v>-1.97191580236399E-2</v>
+      </c>
+      <c r="I29" s="26">
+        <v>0.60561683952720202</v>
+      </c>
+      <c r="J29" s="27">
+        <v>594172.67650196899</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="33">
+        <f>A29+5%</f>
+        <v>0.1</v>
+      </c>
+      <c r="B30" s="28">
+        <v>-0.14279390292980601</v>
+      </c>
+      <c r="C30" s="28">
+        <v>-8.0859854037432302E-2</v>
+      </c>
+      <c r="D30" s="28">
+        <v>-0.28451053128419102</v>
+      </c>
+      <c r="E30" s="28">
+        <v>5.8589768150356297E-2</v>
+      </c>
+      <c r="F30" s="28">
+        <v>-5.6601897826202303E-3</v>
+      </c>
+      <c r="G30" s="28">
+        <v>-1.42255265642096E-2</v>
+      </c>
+      <c r="H30" s="28">
+        <v>-3.7645665317857999E-2</v>
+      </c>
+      <c r="I30" s="28">
+        <v>0.62354334682141999</v>
+      </c>
+      <c r="J30" s="29">
+        <v>1188345.3530039401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="32">
+        <f t="shared" ref="A31:A48" si="1">A30+5%</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="B31" s="26">
+        <v>-0.214190854394709</v>
+      </c>
+      <c r="C31" s="26">
+        <v>-0.121289781056148</v>
+      </c>
+      <c r="D31" s="26">
+        <v>-0.42676579692628602</v>
+      </c>
+      <c r="E31" s="26">
+        <v>8.7884652225534293E-2</v>
+      </c>
+      <c r="F31" s="26">
+        <v>-8.4902846739303497E-3</v>
+      </c>
+      <c r="G31" s="26">
+        <v>-2.13382898463143E-2</v>
+      </c>
+      <c r="H31" s="26">
+        <v>-5.4013345890839601E-2</v>
+      </c>
+      <c r="I31" s="26">
+        <v>0.63991102739440198</v>
+      </c>
+      <c r="J31" s="27">
+        <v>1782518.0295059001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="33">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="B32" s="28">
+        <v>-0.28558780585961202</v>
+      </c>
+      <c r="C32" s="28">
+        <v>-0.16171970807486499</v>
+      </c>
+      <c r="D32" s="28">
+        <v>-0.56902106256838303</v>
+      </c>
+      <c r="E32" s="28">
+        <v>0.117179536300712</v>
+      </c>
+      <c r="F32" s="28">
+        <v>-1.13203795652405E-2</v>
+      </c>
+      <c r="G32" s="28">
+        <v>-2.8451053128419099E-2</v>
+      </c>
+      <c r="H32" s="28">
+        <v>-6.9017053082739699E-2</v>
+      </c>
+      <c r="I32" s="28">
+        <v>0.65491473458630201</v>
+      </c>
+      <c r="J32" s="29">
+        <v>2376690.7060078802</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="32">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="B33" s="26">
+        <v>-0.35698475732451501</v>
+      </c>
+      <c r="C33" s="26">
+        <v>-0.202149635093581</v>
+      </c>
+      <c r="D33" s="26">
+        <v>-0.71127632821047804</v>
+      </c>
+      <c r="E33" s="26">
+        <v>0.14647442037589101</v>
+      </c>
+      <c r="F33" s="26">
+        <v>-1.4150474456550601E-2</v>
+      </c>
+      <c r="G33" s="26">
+        <v>-3.5563816410523898E-2</v>
+      </c>
+      <c r="H33" s="26">
+        <v>-8.2820463699287597E-2</v>
+      </c>
+      <c r="I33" s="26">
+        <v>0.66871814520285</v>
+      </c>
+      <c r="J33" s="27">
+        <v>2970863.3825098402</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="33">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="B34" s="28">
+        <v>-0.428381708789419</v>
+      </c>
+      <c r="C34" s="28">
+        <v>-0.242579562112297</v>
+      </c>
+      <c r="D34" s="28">
+        <v>-0.85353159385257404</v>
+      </c>
+      <c r="E34" s="28">
+        <v>0.175769304451069</v>
+      </c>
+      <c r="F34" s="28">
+        <v>-1.69805693478608E-2</v>
+      </c>
+      <c r="G34" s="28">
+        <v>-4.2676579692628697E-2</v>
+      </c>
+      <c r="H34" s="28">
+        <v>-9.5562073499178002E-2</v>
+      </c>
+      <c r="I34" s="28">
+        <v>0.68145975500274003</v>
+      </c>
+      <c r="J34" s="29">
+        <v>3565036.05901181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="32">
+        <f t="shared" si="1"/>
+        <v>0.35</v>
+      </c>
+      <c r="B35" s="26">
+        <v>-0.49977866025432199</v>
+      </c>
+      <c r="C35" s="26">
+        <v>-0.28300948913101398</v>
+      </c>
+      <c r="D35" s="26">
+        <v>-0.99578685949467005</v>
+      </c>
+      <c r="E35" s="26">
+        <v>0.205064188526247</v>
+      </c>
+      <c r="F35" s="26">
+        <v>-1.98106642391709E-2</v>
+      </c>
+      <c r="G35" s="26">
+        <v>-4.9789342974733503E-2</v>
+      </c>
+      <c r="H35" s="26">
+        <v>-0.107359860350928</v>
+      </c>
+      <c r="I35" s="26">
+        <v>0.69325754185448996</v>
+      </c>
+      <c r="J35" s="27">
+        <v>4159208.7355137798</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="33">
+        <f t="shared" si="1"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="B36" s="28">
+        <v>-0.57117561171922504</v>
+      </c>
+      <c r="C36" s="28">
+        <v>-0.32343941614972999</v>
+      </c>
+      <c r="D36" s="28">
+        <v>-1.1380421251367701</v>
+      </c>
+      <c r="E36" s="28">
+        <v>0.23435907260142499</v>
+      </c>
+      <c r="F36" s="28">
+        <v>-2.2640759130481102E-2</v>
+      </c>
+      <c r="G36" s="28">
+        <v>-5.6902106256838302E-2</v>
+      </c>
+      <c r="H36" s="28">
+        <v>-0.118314948141839</v>
+      </c>
+      <c r="I36" s="28">
+        <v>0.70421262964540099</v>
+      </c>
+      <c r="J36" s="29">
+        <v>4753381.4120157501</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="32">
+        <f t="shared" si="1"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="B37" s="26">
+        <v>-0.64257256318412803</v>
+      </c>
+      <c r="C37" s="26">
+        <v>-0.36386934316844599</v>
+      </c>
+      <c r="D37" s="26">
+        <v>-1.28029739077886</v>
+      </c>
+      <c r="E37" s="26">
+        <v>0.26365395667660302</v>
+      </c>
+      <c r="F37" s="26">
+        <v>-2.5470854021791198E-2</v>
+      </c>
+      <c r="G37" s="26">
+        <v>-6.4014869538943101E-2</v>
+      </c>
+      <c r="H37" s="26">
+        <v>-0.12851451263682601</v>
+      </c>
+      <c r="I37" s="26">
+        <v>0.71441219414038803</v>
+      </c>
+      <c r="J37" s="27">
+        <v>5347554.0885177199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="33">
+        <f t="shared" si="1"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="B38" s="28">
+        <v>-0.71396951464903102</v>
+      </c>
+      <c r="C38" s="28">
+        <v>-0.404299270187162</v>
+      </c>
+      <c r="D38" s="28">
+        <v>-1.4225526564209601</v>
+      </c>
+      <c r="E38" s="28">
+        <v>0.29294884075178101</v>
+      </c>
+      <c r="F38" s="28">
+        <v>-2.8300948913101299E-2</v>
+      </c>
+      <c r="G38" s="28">
+        <v>-7.1127632821047795E-2</v>
+      </c>
+      <c r="H38" s="28">
+        <v>-0.13803410616547901</v>
+      </c>
+      <c r="I38" s="28">
+        <v>0.72393178766904098</v>
+      </c>
+      <c r="J38" s="29">
+        <v>5941726.7650196897</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="32">
+        <f t="shared" si="1"/>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="B39" s="26">
+        <v>-0.78536646611393401</v>
+      </c>
+      <c r="C39" s="26">
+        <v>-0.444729197205879</v>
+      </c>
+      <c r="D39" s="26">
+        <v>-1.56480792206305</v>
+      </c>
+      <c r="E39" s="26">
+        <v>0.32224372482695901</v>
+      </c>
+      <c r="F39" s="26">
+        <v>-3.11310438044115E-2</v>
+      </c>
+      <c r="G39" s="26">
+        <v>-7.8240396103152601E-2</v>
+      </c>
+      <c r="H39" s="26">
+        <v>-0.146939532369704</v>
+      </c>
+      <c r="I39" s="26">
+        <v>0.73283721387326595</v>
+      </c>
+      <c r="J39" s="27">
+        <v>6535899.4415216502</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="33">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="B40" s="28">
+        <v>-0.85676341757883701</v>
+      </c>
+      <c r="C40" s="28">
+        <v>-0.48515912422459501</v>
+      </c>
+      <c r="D40" s="28">
+        <v>-1.7070631877051501</v>
+      </c>
+      <c r="E40" s="28">
+        <v>0.35153860890213701</v>
+      </c>
+      <c r="F40" s="28">
+        <v>-3.39611386957216E-2</v>
+      </c>
+      <c r="G40" s="28">
+        <v>-8.5353159385257393E-2</v>
+      </c>
+      <c r="H40" s="28">
+        <v>-0.155288369436164</v>
+      </c>
+      <c r="I40" s="28">
+        <v>0.741186050939726</v>
+      </c>
+      <c r="J40" s="29">
+        <v>7130072.1180236302</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="32">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="B41" s="26">
+        <v>-0.92816036904374</v>
+      </c>
+      <c r="C41" s="26">
+        <v>-0.52558905124331101</v>
+      </c>
+      <c r="D41" s="26">
+        <v>-1.84931845334724</v>
+      </c>
+      <c r="E41" s="26">
+        <v>0.380833492977315</v>
+      </c>
+      <c r="F41" s="26">
+        <v>-3.6791233587031798E-2</v>
+      </c>
+      <c r="G41" s="26">
+        <v>-9.2465922667362199E-2</v>
+      </c>
+      <c r="H41" s="26">
+        <v>-0.16313121637738501</v>
+      </c>
+      <c r="I41" s="26">
+        <v>0.74902889788094695</v>
+      </c>
+      <c r="J41" s="27">
+        <v>7724244.7945256</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="33">
+        <f t="shared" si="1"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="B42" s="28">
+        <v>-0.99955732050864299</v>
+      </c>
+      <c r="C42" s="28">
+        <v>-0.56601897826202696</v>
+      </c>
+      <c r="D42" s="28">
+        <v>-1.9915737189893401</v>
+      </c>
+      <c r="E42" s="28">
+        <v>0.410128377052493</v>
+      </c>
+      <c r="F42" s="28">
+        <v>-3.9621328478341898E-2</v>
+      </c>
+      <c r="G42" s="28">
+        <v>-9.9578685949467005E-2</v>
+      </c>
+      <c r="H42" s="28">
+        <v>-0.170512719380886</v>
+      </c>
+      <c r="I42" s="28">
+        <v>0.756410400884448</v>
+      </c>
+      <c r="J42" s="29">
+        <v>8318417.4710275596</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="32">
+        <f t="shared" si="1"/>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="B43" s="26">
+        <v>-1.0709542719735501</v>
+      </c>
+      <c r="C43" s="26">
+        <v>-0.60644890528074402</v>
+      </c>
+      <c r="D43" s="26">
+        <v>-2.1338289846314402</v>
+      </c>
+      <c r="E43" s="26">
+        <v>0.43942326112767199</v>
+      </c>
+      <c r="F43" s="26">
+        <v>-4.2451423369652103E-2</v>
+      </c>
+      <c r="G43" s="26">
+        <v>-0.10669144923157201</v>
+      </c>
+      <c r="H43" s="26">
+        <v>-0.177472422212759</v>
+      </c>
+      <c r="I43" s="26">
+        <v>0.76337010371632097</v>
+      </c>
+      <c r="J43" s="27">
+        <v>8912590.1475295294</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="33">
+        <f t="shared" si="1"/>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="B44" s="28">
+        <v>-1.1423512234384501</v>
+      </c>
+      <c r="C44" s="28">
+        <v>-0.64687883229945997</v>
+      </c>
+      <c r="D44" s="28">
+        <v>-2.2760842502735299</v>
+      </c>
+      <c r="E44" s="28">
+        <v>0.46871814520284999</v>
+      </c>
+      <c r="F44" s="28">
+        <v>-4.5281518260962203E-2</v>
+      </c>
+      <c r="G44" s="28">
+        <v>-0.11380421251367701</v>
+      </c>
+      <c r="H44" s="28">
+        <v>-0.18404547488730599</v>
+      </c>
+      <c r="I44" s="28">
+        <v>0.76994315639086797</v>
+      </c>
+      <c r="J44" s="29">
+        <v>9506762.8240315001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="32">
+        <f t="shared" si="1"/>
+        <v>0.8500000000000002</v>
+      </c>
+      <c r="B45" s="26">
+        <v>-1.2137481749033501</v>
+      </c>
+      <c r="C45" s="26">
+        <v>-0.68730875931817603</v>
+      </c>
+      <c r="D45" s="26">
+        <v>-2.4183395159156298</v>
+      </c>
+      <c r="E45" s="26">
+        <v>0.49801302927802799</v>
+      </c>
+      <c r="F45" s="26">
+        <v>-4.8111613152272303E-2</v>
+      </c>
+      <c r="G45" s="26">
+        <v>-0.12091697579578101</v>
+      </c>
+      <c r="H45" s="26">
+        <v>-0.19026322741728199</v>
+      </c>
+      <c r="I45" s="26">
+        <v>0.77616090892084399</v>
+      </c>
+      <c r="J45" s="27">
+        <v>10100935.500533501</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="33">
+        <f t="shared" si="1"/>
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="B46" s="28">
+        <v>-1.2851451263682601</v>
+      </c>
+      <c r="C46" s="28">
+        <v>-0.72773868633689198</v>
+      </c>
+      <c r="D46" s="28">
+        <v>-2.5605947815577199</v>
+      </c>
+      <c r="E46" s="28">
+        <v>0.52730791335320604</v>
+      </c>
+      <c r="F46" s="28">
+        <v>-5.0941708043582501E-2</v>
+      </c>
+      <c r="G46" s="28">
+        <v>-0.12802973907788601</v>
+      </c>
+      <c r="H46" s="28">
+        <v>-0.19615372981410201</v>
+      </c>
+      <c r="I46" s="28">
+        <v>0.78205141131766398</v>
+      </c>
+      <c r="J46" s="29">
+        <v>10695108.177035401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="32">
+        <f t="shared" si="1"/>
+        <v>0.95000000000000029</v>
+      </c>
+      <c r="B47" s="26">
+        <v>-1.3565420778331601</v>
+      </c>
+      <c r="C47" s="26">
+        <v>-0.76816861335560904</v>
+      </c>
+      <c r="D47" s="26">
+        <v>-2.7028500471998198</v>
+      </c>
+      <c r="E47" s="26">
+        <v>0.55660279742838403</v>
+      </c>
+      <c r="F47" s="26">
+        <v>-5.3771802934892601E-2</v>
+      </c>
+      <c r="G47" s="26">
+        <v>-0.13514250235999101</v>
+      </c>
+      <c r="H47" s="26">
+        <v>-0.20174215516493099</v>
+      </c>
+      <c r="I47" s="26">
+        <v>0.78763983666849302</v>
+      </c>
+      <c r="J47" s="27">
+        <v>11289280.853537399</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="33">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="B48" s="28">
+        <v>-1.42793902929806</v>
+      </c>
+      <c r="C48" s="28">
+        <v>-0.80859854037432499</v>
+      </c>
+      <c r="D48" s="28">
+        <v>-2.8451053128419099</v>
+      </c>
+      <c r="E48" s="28">
+        <v>0.58589768150356203</v>
+      </c>
+      <c r="F48" s="28">
+        <v>-5.6601897826202702E-2</v>
+      </c>
+      <c r="G48" s="28">
+        <v>-0.14225526564209601</v>
+      </c>
+      <c r="H48" s="28">
+        <v>-0.20705115924821901</v>
+      </c>
+      <c r="I48" s="28">
+        <v>0.79294884075178096</v>
+      </c>
+      <c r="J48" s="29">
+        <v>11883453.5300394</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+    </row>
+    <row r="52" spans="1:10" ht="38.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I52" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="J52" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="B54" s="26">
+        <v>-5.0897863152406901E-2</v>
+      </c>
+      <c r="C54" s="26">
+        <v>2.0484214097779702E-2</v>
+      </c>
+      <c r="D54" s="26">
+        <v>-4.3125736187924799E-2</v>
+      </c>
+      <c r="E54" s="26">
+        <v>3.5239619685801998E-2</v>
+      </c>
+      <c r="F54" s="26">
+        <v>1.4338949868446299E-3</v>
+      </c>
+      <c r="G54" s="26">
+        <v>-2.1562868093962101E-3</v>
+      </c>
+      <c r="H54" s="26">
+        <v>-1.4057505061141E-2</v>
+      </c>
+      <c r="I54" s="26">
+        <v>0.71884989877717997</v>
+      </c>
+      <c r="J54" s="27">
+        <v>833475.41760162194</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="33">
+        <f>A54+5%</f>
+        <v>0.1</v>
+      </c>
+      <c r="B55" s="28">
+        <v>-0.101795726304814</v>
+      </c>
+      <c r="C55" s="28">
+        <v>4.0968428195560201E-2</v>
+      </c>
+      <c r="D55" s="28">
+        <v>-8.6251472375850097E-2</v>
+      </c>
+      <c r="E55" s="28">
+        <v>7.0479239371604094E-2</v>
+      </c>
+      <c r="F55" s="28">
+        <v>2.8677899736892099E-3</v>
+      </c>
+      <c r="G55" s="28">
+        <v>-4.3125736187925E-3</v>
+      </c>
+      <c r="H55" s="28">
+        <v>-2.6837055116723699E-2</v>
+      </c>
+      <c r="I55" s="28">
+        <v>0.73162944883276304</v>
+      </c>
+      <c r="J55" s="29">
+        <v>1666950.8352032399</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="32">
+        <f t="shared" ref="A56:A73" si="2">A55+5%</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="B56" s="26">
+        <v>-0.152693589457221</v>
+      </c>
+      <c r="C56" s="26">
+        <v>6.1452642293340201E-2</v>
+      </c>
+      <c r="D56" s="26">
+        <v>-0.12937720856377499</v>
+      </c>
+      <c r="E56" s="26">
+        <v>0.10571885905740599</v>
+      </c>
+      <c r="F56" s="26">
+        <v>4.3016849605337802E-3</v>
+      </c>
+      <c r="G56" s="26">
+        <v>-6.4688604281887101E-3</v>
+      </c>
+      <c r="H56" s="26">
+        <v>-3.8505339950081797E-2</v>
+      </c>
+      <c r="I56" s="26">
+        <v>0.74329773366612095</v>
+      </c>
+      <c r="J56" s="27">
+        <v>2500426.25280486</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="33">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="B57" s="28">
+        <v>-0.20359145260962799</v>
+      </c>
+      <c r="C57" s="28">
+        <v>8.1936856391120097E-2</v>
+      </c>
+      <c r="D57" s="28">
+        <v>-0.1725029447517</v>
+      </c>
+      <c r="E57" s="28">
+        <v>0.14095847874320799</v>
+      </c>
+      <c r="F57" s="28">
+        <v>5.7355799473784198E-3</v>
+      </c>
+      <c r="G57" s="28">
+        <v>-8.6251472375849896E-3</v>
+      </c>
+      <c r="H57" s="28">
+        <v>-4.9201267713993503E-2</v>
+      </c>
+      <c r="I57" s="28">
+        <v>0.75399366143003299</v>
+      </c>
+      <c r="J57" s="29">
+        <v>3333901.6704064901</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="32">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="B58" s="26">
+        <v>-0.25448931576203498</v>
+      </c>
+      <c r="C58" s="26">
+        <v>0.10242107048890001</v>
+      </c>
+      <c r="D58" s="26">
+        <v>-0.21562868093962501</v>
+      </c>
+      <c r="E58" s="26">
+        <v>0.17619809842900999</v>
+      </c>
+      <c r="F58" s="26">
+        <v>7.1694749342229901E-3</v>
+      </c>
+      <c r="G58" s="26">
+        <v>-1.07814340469813E-2</v>
+      </c>
+      <c r="H58" s="26">
+        <v>-5.9041521256792101E-2</v>
+      </c>
+      <c r="I58" s="26">
+        <v>0.76383391497283204</v>
+      </c>
+      <c r="J58" s="27">
+        <v>4167377.0880081099</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="33">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="B59" s="28">
+        <v>-0.305387178914442</v>
+      </c>
+      <c r="C59" s="28">
+        <v>0.12290528458668</v>
+      </c>
+      <c r="D59" s="28">
+        <v>-0.25875441712755098</v>
+      </c>
+      <c r="E59" s="28">
+        <v>0.21143771811481199</v>
+      </c>
+      <c r="F59" s="28">
+        <v>8.6033699210675708E-3</v>
+      </c>
+      <c r="G59" s="28">
+        <v>-1.29377208563775E-2</v>
+      </c>
+      <c r="H59" s="28">
+        <v>-6.81248322193755E-2</v>
+      </c>
+      <c r="I59" s="28">
+        <v>0.77291722593541501</v>
+      </c>
+      <c r="J59" s="29">
+        <v>5000852.5056097303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="32">
+        <f t="shared" si="2"/>
+        <v>0.35</v>
+      </c>
+      <c r="B60" s="26">
+        <v>-0.35628504206684902</v>
+      </c>
+      <c r="C60" s="26">
+        <v>0.14338949868445999</v>
+      </c>
+      <c r="D60" s="26">
+        <v>-0.30188015331547602</v>
+      </c>
+      <c r="E60" s="26">
+        <v>0.24667733780061399</v>
+      </c>
+      <c r="F60" s="26">
+        <v>1.00372649079123E-2</v>
+      </c>
+      <c r="G60" s="26">
+        <v>-1.50940076657738E-2</v>
+      </c>
+      <c r="H60" s="26">
+        <v>-7.6535305332878695E-2</v>
+      </c>
+      <c r="I60" s="26">
+        <v>0.78132769904891797</v>
+      </c>
+      <c r="J60" s="27">
+        <v>5834327.9232113604</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="33">
+        <f t="shared" si="2"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="B61" s="28">
+        <v>-0.40718290521925599</v>
+      </c>
+      <c r="C61" s="28">
+        <v>0.16387371278224</v>
+      </c>
+      <c r="D61" s="28">
+        <v>-0.345005889503401</v>
+      </c>
+      <c r="E61" s="28">
+        <v>0.28191695748641599</v>
+      </c>
+      <c r="F61" s="28">
+        <v>1.14711598947568E-2</v>
+      </c>
+      <c r="G61" s="28">
+        <v>-1.725029447517E-2</v>
+      </c>
+      <c r="H61" s="28">
+        <v>-8.4345030366845902E-2</v>
+      </c>
+      <c r="I61" s="28">
+        <v>0.78913742408288501</v>
+      </c>
+      <c r="J61" s="29">
+        <v>6667803.34081297</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="32">
+        <f t="shared" si="2"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="B62" s="26">
+        <v>-0.45808076837166301</v>
+      </c>
+      <c r="C62" s="26">
+        <v>0.18435792688002001</v>
+      </c>
+      <c r="D62" s="26">
+        <v>-0.38813162569132598</v>
+      </c>
+      <c r="E62" s="26">
+        <v>0.31715657717221801</v>
+      </c>
+      <c r="F62" s="26">
+        <v>1.2905054881601499E-2</v>
+      </c>
+      <c r="G62" s="26">
+        <v>-1.94065812845663E-2</v>
+      </c>
+      <c r="H62" s="26">
+        <v>-9.1616153674332707E-2</v>
+      </c>
+      <c r="I62" s="26">
+        <v>0.79640854739037203</v>
+      </c>
+      <c r="J62" s="27">
+        <v>7501278.7584145898</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="33">
+        <f t="shared" si="2"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="B63" s="28">
+        <v>-0.50897863152406997</v>
+      </c>
+      <c r="C63" s="28">
+        <v>0.20484214097780001</v>
+      </c>
+      <c r="D63" s="28">
+        <v>-0.43125736187925101</v>
+      </c>
+      <c r="E63" s="28">
+        <v>0.35239619685801998</v>
+      </c>
+      <c r="F63" s="28">
+        <v>1.4338949868445999E-2</v>
+      </c>
+      <c r="G63" s="28">
+        <v>-2.1562868093962601E-2</v>
+      </c>
+      <c r="H63" s="28">
+        <v>-9.8402535427986895E-2</v>
+      </c>
+      <c r="I63" s="28">
+        <v>0.80319492914402602</v>
+      </c>
+      <c r="J63" s="29">
+        <v>8334754.1760162199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="32">
+        <f t="shared" si="2"/>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="B64" s="26">
+        <v>-0.55987649467647704</v>
+      </c>
+      <c r="C64" s="26">
+        <v>0.22532635507557999</v>
+      </c>
+      <c r="D64" s="26">
+        <v>-0.47438309806717599</v>
+      </c>
+      <c r="E64" s="26">
+        <v>0.38763581654382201</v>
+      </c>
+      <c r="F64" s="26">
+        <v>1.57728448552906E-2</v>
+      </c>
+      <c r="G64" s="26">
+        <v>-2.37191549033588E-2</v>
+      </c>
+      <c r="H64" s="26">
+        <v>-0.10475108610076</v>
+      </c>
+      <c r="I64" s="26">
+        <v>0.80954347981679997</v>
+      </c>
+      <c r="J64" s="27">
+        <v>9168229.5936178397</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="33">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="B65" s="28">
+        <v>-0.61077435782888401</v>
+      </c>
+      <c r="C65" s="28">
+        <v>0.24581056917336</v>
+      </c>
+      <c r="D65" s="28">
+        <v>-0.51750883425510097</v>
+      </c>
+      <c r="E65" s="28">
+        <v>0.42287543622962398</v>
+      </c>
+      <c r="F65" s="28">
+        <v>1.7206739842135301E-2</v>
+      </c>
+      <c r="G65" s="28">
+        <v>-2.58754417127551E-2</v>
+      </c>
+      <c r="H65" s="28">
+        <v>-0.110702852356485</v>
+      </c>
+      <c r="I65" s="28">
+        <v>0.81549524607252499</v>
+      </c>
+      <c r="J65" s="29">
+        <v>10001705.0112195</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="32">
+        <f t="shared" si="2"/>
+        <v>0.65</v>
+      </c>
+      <c r="B66" s="26">
+        <v>-0.66167222098129097</v>
+      </c>
+      <c r="C66" s="26">
+        <v>0.26629478327113998</v>
+      </c>
+      <c r="D66" s="26">
+        <v>-0.560634570443026</v>
+      </c>
+      <c r="E66" s="26">
+        <v>0.45811505591542501</v>
+      </c>
+      <c r="F66" s="26">
+        <v>1.8640634828979801E-2</v>
+      </c>
+      <c r="G66" s="26">
+        <v>-2.80317285221513E-2</v>
+      </c>
+      <c r="H66" s="26">
+        <v>-0.116293905505803</v>
+      </c>
+      <c r="I66" s="26">
+        <v>0.82108629922184195</v>
+      </c>
+      <c r="J66" s="27">
+        <v>10835180.4288211</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="33">
+        <f t="shared" si="2"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="B67" s="28">
+        <v>-0.71257008413369805</v>
+      </c>
+      <c r="C67" s="28">
+        <v>0.28677899736891999</v>
+      </c>
+      <c r="D67" s="28">
+        <v>-0.60376030663095204</v>
+      </c>
+      <c r="E67" s="28">
+        <v>0.49335467560122798</v>
+      </c>
+      <c r="F67" s="28">
+        <v>2.0074529815824499E-2</v>
+      </c>
+      <c r="G67" s="28">
+        <v>-3.01880153315476E-2</v>
+      </c>
+      <c r="H67" s="28">
+        <v>-0.121556073175749</v>
+      </c>
+      <c r="I67" s="28">
+        <v>0.82634846689178798</v>
+      </c>
+      <c r="J67" s="29">
+        <v>11668655.8464227</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="32">
+        <f t="shared" si="2"/>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="B68" s="26">
+        <v>-0.76346794728610501</v>
+      </c>
+      <c r="C68" s="26">
+        <v>0.30726321146669999</v>
+      </c>
+      <c r="D68" s="26">
+        <v>-0.64688604281887696</v>
+      </c>
+      <c r="E68" s="26">
+        <v>0.52859429528702995</v>
+      </c>
+      <c r="F68" s="26">
+        <v>2.1508424802668999E-2</v>
+      </c>
+      <c r="G68" s="26">
+        <v>-3.2344302140943797E-2</v>
+      </c>
+      <c r="H68" s="26">
+        <v>-0.12651754555026901</v>
+      </c>
+      <c r="I68" s="26">
+        <v>0.83130993926630803</v>
+      </c>
+      <c r="J68" s="27">
+        <v>12502131.264024301</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="33">
+        <f t="shared" si="2"/>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="B69" s="28">
+        <v>-0.81436581043851197</v>
+      </c>
+      <c r="C69" s="28">
+        <v>0.32774742556448</v>
+      </c>
+      <c r="D69" s="28">
+        <v>-0.690011779006802</v>
+      </c>
+      <c r="E69" s="28">
+        <v>0.56383391497283197</v>
+      </c>
+      <c r="F69" s="28">
+        <v>2.29423197895136E-2</v>
+      </c>
+      <c r="G69" s="28">
+        <v>-3.4500588950340097E-2</v>
+      </c>
+      <c r="H69" s="28">
+        <v>-0.13120338057064901</v>
+      </c>
+      <c r="I69" s="28">
+        <v>0.83599577428668903</v>
+      </c>
+      <c r="J69" s="29">
+        <v>13335606.681625901</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="32">
+        <f t="shared" si="2"/>
+        <v>0.8500000000000002</v>
+      </c>
+      <c r="B70" s="26">
+        <v>-0.86526367359091905</v>
+      </c>
+      <c r="C70" s="26">
+        <v>0.34823163966226001</v>
+      </c>
+      <c r="D70" s="26">
+        <v>-0.73313751519472703</v>
+      </c>
+      <c r="E70" s="26">
+        <v>0.599073534658633</v>
+      </c>
+      <c r="F70" s="26">
+        <v>2.43762147763582E-2</v>
+      </c>
+      <c r="G70" s="26">
+        <v>-3.66568757597363E-2</v>
+      </c>
+      <c r="H70" s="26">
+        <v>-0.13563592721154999</v>
+      </c>
+      <c r="I70" s="26">
+        <v>0.84042832092758901</v>
+      </c>
+      <c r="J70" s="27">
+        <v>14169082.0992276</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="33">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="B71" s="28">
+        <v>-0.91616153674332601</v>
+      </c>
+      <c r="C71" s="28">
+        <v>0.36871585376004001</v>
+      </c>
+      <c r="D71" s="28">
+        <v>-0.77626325138265195</v>
+      </c>
+      <c r="E71" s="28">
+        <v>0.63431315434443503</v>
+      </c>
+      <c r="F71" s="28">
+        <v>2.5810109763202801E-2</v>
+      </c>
+      <c r="G71" s="28">
+        <v>-3.88131625691326E-2</v>
+      </c>
+      <c r="H71" s="28">
+        <v>-0.13983518192398101</v>
+      </c>
+      <c r="I71" s="28">
+        <v>0.844627575640021</v>
+      </c>
+      <c r="J71" s="29">
+        <v>15002557.5168292</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="32">
+        <f t="shared" si="2"/>
+        <v>0.95000000000000029</v>
+      </c>
+      <c r="B72" s="26">
+        <v>-0.96705939989573297</v>
+      </c>
+      <c r="C72" s="26">
+        <v>0.38920006785782002</v>
+      </c>
+      <c r="D72" s="26">
+        <v>-0.81938898757057699</v>
+      </c>
+      <c r="E72" s="26">
+        <v>0.66955277403023705</v>
+      </c>
+      <c r="F72" s="26">
+        <v>2.7244004750047499E-2</v>
+      </c>
+      <c r="G72" s="26">
+        <v>-4.0969449378528797E-2</v>
+      </c>
+      <c r="H72" s="26">
+        <v>-0.143819090240904</v>
+      </c>
+      <c r="I72" s="26">
+        <v>0.84861148395694297</v>
+      </c>
+      <c r="J72" s="27">
+        <v>15836032.9344308</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="33">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="B73" s="28">
+        <v>-1.0179572630481399</v>
+      </c>
+      <c r="C73" s="28">
+        <v>0.40968428195560003</v>
+      </c>
+      <c r="D73" s="28">
+        <v>-0.86251472375850302</v>
+      </c>
+      <c r="E73" s="28">
+        <v>0.70479239371603897</v>
+      </c>
+      <c r="F73" s="28">
+        <v>2.8677899736891999E-2</v>
+      </c>
+      <c r="G73" s="28">
+        <v>-4.3125736187925097E-2</v>
+      </c>
+      <c r="H73" s="28">
+        <v>-0.14760380314197999</v>
+      </c>
+      <c r="I73" s="28">
+        <v>0.85239619685802004</v>
+      </c>
+      <c r="J73" s="29">
+        <v>16669508.352032401</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A51:J51"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>